<commit_message>
Still fighting with session tokens
I really should have just stuck to fixing the search...
</commit_message>
<xml_diff>
--- a/Progress Tracker.xlsx
+++ b/Progress Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdgl-my.sharepoint.com/personal/rlo_blackdiamondgroup_com/Documents/Main Projects/GLPI-search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B608C54A-ACA5-471B-8099-6E63BD2B81FC}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D86EC8C9-B6D7-4C41-A755-023EAEA5094F}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
   </bookViews>
@@ -117,9 +117,6 @@
     <t>Site icon</t>
   </si>
   <si>
-    <t>Store session info</t>
-  </si>
-  <si>
     <t>COMPLETION DATE</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Searching via service tag</t>
+  </si>
+  <si>
+    <t>Store session token info</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -695,7 +695,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +767,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -786,7 +786,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Added search bar, ID no longer hard coded, UI  changes
I win.
</commit_message>
<xml_diff>
--- a/Progress Tracker.xlsx
+++ b/Progress Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdgl-my.sharepoint.com/personal/rlo_blackdiamondgroup_com/Documents/Main Projects/GLPI-search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D86EC8C9-B6D7-4C41-A755-023EAEA5094F}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15C9B231-E0BD-4282-9C6F-3C63053FAE4F}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
+    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Front End" sheetId="1" r:id="rId1"/>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60981241-097C-4D7C-A446-9062E4E45EE4}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E63138-A7FA-4E56-8473-657B5DB99540}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +781,10 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45079</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,6 +793,9 @@
       </c>
       <c r="B9" t="s">
         <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45076</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Can now save several devices to CSV
</commit_message>
<xml_diff>
--- a/Progress Tracker.xlsx
+++ b/Progress Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdgl-my.sharepoint.com/personal/rlo_blackdiamondgroup_com/Documents/Main Projects/GLPI-search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15C9B231-E0BD-4282-9C6F-3C63053FAE4F}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F9453E4-C23A-41D7-8189-3B9AD796E0C7}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
+    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Front End" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -96,9 +96,6 @@
     <t>app token enter</t>
   </si>
   <si>
-    <t>IN PROGRESS</t>
-  </si>
-  <si>
     <t>BASIC UI</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Store session token info</t>
+  </si>
+  <si>
+    <t>Data table</t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -554,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60981241-097C-4D7C-A446-9062E4E45EE4}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,12 +633,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -597,7 +657,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45079</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -605,7 +668,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45079</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -619,14 +685,25 @@
         <v>45076</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45079</v>
+      </c>
+    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -634,7 +711,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -642,15 +719,18 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>45079</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -673,15 +753,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B22">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"INCOMPLETE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B22">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"COMPLETE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -694,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E63138-A7FA-4E56-8473-657B5DB99540}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +847,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -778,7 +858,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -789,7 +869,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -800,10 +880,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>45079</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -827,18 +910,52 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2">
+        <v>45079</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45079</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B14:B15 B3:B10">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"COMPLETE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"INCOMPLETE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"COMPLETE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"INCOMPLETE"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added columns for screen size and notes
</commit_message>
<xml_diff>
--- a/Progress Tracker.xlsx
+++ b/Progress Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdgl-my.sharepoint.com/personal/rlo_blackdiamondgroup_com/Documents/Main Projects/GLPI-search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A2384A1-67ED-4AAB-A59D-47AEEAFD7FE3}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4FC15AB-A348-4116-AAD2-48DF2C865534}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-18740" yWindow="470" windowWidth="16420" windowHeight="10150" activeTab="2" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
+    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
   </bookViews>
   <sheets>
     <sheet name="App Dev Log" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
     <t>BAD</t>
   </si>
   <si>
-    <t>Bad battery, needs replacing; Keyboard has cosmetic damage on ENT, A, S, N</t>
+    <t>Bad battery, needs replacing; Keyboard has cosmetic damage on Enter, A, S, N</t>
   </si>
 </sst>
 </file>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60981241-097C-4D7C-A446-9062E4E45EE4}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,7 +2538,7 @@
   <dimension ref="A1:H121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Exception handling for 0 or 2+ drives/memory/cpu
Changed calling HDD, RAM, and CPU key from all at once to one at a time as needed in order to account for edge cases. Also fixed the export button to not duplicate.
</commit_message>
<xml_diff>
--- a/Progress Tracker.xlsx
+++ b/Progress Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdgl-my.sharepoint.com/personal/rlo_blackdiamondgroup_com/Documents/Main Projects/GLPI-search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4FC15AB-A348-4116-AAD2-48DF2C865534}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F1BF58F-030B-4C42-86BB-60726C528F3E}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
+    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
   </bookViews>
   <sheets>
     <sheet name="App Dev Log" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="47">
   <si>
     <t>Task</t>
   </si>
@@ -167,6 +167,21 @@
   </si>
   <si>
     <t>Bad battery, needs replacing; Keyboard has cosmetic damage on Enter, A, S, N</t>
+  </si>
+  <si>
+    <t>Notes - Screen size and general</t>
+  </si>
+  <si>
+    <t>Stability</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>Accounting for 0 or 2+ drives</t>
+  </si>
+  <si>
+    <t>Export button not duplicating</t>
   </si>
 </sst>
 </file>
@@ -227,7 +242,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -245,6 +260,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -285,6 +320,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -496,6 +541,370 @@
           </cell>
           <cell r="G3">
             <v>13.3</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>FJ9QLQ2</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>Latitude 5490</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E4">
+            <v>8192</v>
+          </cell>
+          <cell r="F4" t="str">
+            <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
+          </cell>
+          <cell r="G4">
+            <v>13.3</v>
+          </cell>
+          <cell r="H4" t="str">
+            <v>No battery; bad trackpad</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>H4RFJR2</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>Latitude 5490</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E5">
+            <v>8192</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
+          </cell>
+          <cell r="G5">
+            <v>13.3</v>
+          </cell>
+          <cell r="H5" t="str">
+            <v>Bad battery; random shutdowns; no esc key</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>BBMJLQ2</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>Latitude 5490</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E6">
+            <v>8192</v>
+          </cell>
+          <cell r="F6" t="str">
+            <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
+          </cell>
+          <cell r="G6">
+            <v>13.3</v>
+          </cell>
+          <cell r="H6" t="str">
+            <v>No battery; no hdd</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>HRQBQV2</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>Latitude 5490</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E7">
+            <v>8192</v>
+          </cell>
+          <cell r="F7" t="str">
+            <v>SK hynix SC401 SATA 256GB</v>
+          </cell>
+          <cell r="G7">
+            <v>13.3</v>
+          </cell>
+          <cell r="H7" t="str">
+            <v>No battery; USB-C cosmetic damage</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>C484M12</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>Latitude E6440</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>Intel(R) Core(TM) i5-4310M CPU @ 2.70GHz</v>
+          </cell>
+          <cell r="E8">
+            <v>8192</v>
+          </cell>
+          <cell r="F8" t="str">
+            <v>LITEONIT LCS-180M6S-11 2.5 7mm 180GB</v>
+          </cell>
+          <cell r="G8">
+            <v>13.3</v>
+          </cell>
+          <cell r="H8" t="str">
+            <v>Needs cleaning and check</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>29VM533</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>Latitude 5400</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>Intel(R) Core(TM) i5-8265U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E9">
+            <v>8192</v>
+          </cell>
+          <cell r="F9" t="str">
+            <v>PM991 NVMe Samsung 256GB</v>
+          </cell>
+          <cell r="G9">
+            <v>13.3</v>
+          </cell>
+          <cell r="H9" t="str">
+            <v>No battery; bad screen</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>5DRF3M2</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v>Latitude 5480</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>Intel(R) Core(TM) i5-7200U CPU @ 2.50GHz</v>
+          </cell>
+          <cell r="E10">
+            <v>16384</v>
+          </cell>
+          <cell r="F10" t="str">
+            <v>SK hynix SC308 SATA 128GB</v>
+          </cell>
+          <cell r="G10">
+            <v>13.3</v>
+          </cell>
+          <cell r="H10" t="str">
+            <v>No battery; bad hdd</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>CB8NQQ2</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>Latitude 5490</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E11">
+            <v>8192</v>
+          </cell>
+          <cell r="F11" t="str">
+            <v>SK hynix SC311 SATA 256GB</v>
+          </cell>
+          <cell r="G11">
+            <v>13.3</v>
+          </cell>
+          <cell r="H11" t="str">
+            <v>No battery; no ram; bad keyboard</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>7KW9QQ2</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C12" t="str">
+            <v>Latitude 5490</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E12">
+            <v>8192</v>
+          </cell>
+          <cell r="F12" t="str">
+            <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
+          </cell>
+          <cell r="G12">
+            <v>13.3</v>
+          </cell>
+          <cell r="H12" t="str">
+            <v>No battery; bad keyboard; front cover bulge; bad drivers</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>38MTNN2</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C13" t="str">
+            <v>Latitude 5580</v>
+          </cell>
+          <cell r="D13" t="str">
+            <v>Intel(R) Core(TM) i5-7300U CPU @ 2.60GHz</v>
+          </cell>
+          <cell r="E13">
+            <v>16384</v>
+          </cell>
+          <cell r="F13" t="str">
+            <v>SK hynix SC401 SATA 256GB</v>
+          </cell>
+          <cell r="G13">
+            <v>15.6</v>
+          </cell>
+          <cell r="H13" t="str">
+            <v>No battery; no ram; bad ethernet; ALIAS VMNB0128</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>CVJJMQ2</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C14" t="str">
+            <v>Latitude 5590</v>
+          </cell>
+          <cell r="D14" t="str">
+            <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E14">
+            <v>8192</v>
+          </cell>
+          <cell r="F14" t="str">
+            <v>WDC WD5000LPLX-75ZNTT0</v>
+          </cell>
+          <cell r="G14">
+            <v>15.6</v>
+          </cell>
+          <cell r="H14" t="str">
+            <v>No battery; ALIAS VMNB0131</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>6L6RMQ2</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C15" t="str">
+            <v>Latitude 5490</v>
+          </cell>
+          <cell r="D15" t="str">
+            <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E15">
+            <v>8192</v>
+          </cell>
+          <cell r="F15" t="str">
+            <v>Micron 1100 SATA 256GB</v>
+          </cell>
+          <cell r="G15">
+            <v>13.3</v>
+          </cell>
+          <cell r="H15" t="str">
+            <v>No battery; no j key or joystick; no trackpad buttons</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>H0J05S2</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C16" t="str">
+            <v>Latitude 5490</v>
+          </cell>
+          <cell r="D16" t="str">
+            <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
+          </cell>
+          <cell r="E16">
+            <v>8192</v>
+          </cell>
+          <cell r="F16" t="str">
+            <v>No drive found</v>
+          </cell>
+          <cell r="G16">
+            <v>12.5</v>
+          </cell>
+          <cell r="H16" t="str">
+            <v>Don't even bother</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>JR64Q32</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>Dell Inc.</v>
+          </cell>
+          <cell r="C17" t="str">
+            <v>Latitude E7250</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v>No CPU found</v>
+          </cell>
+          <cell r="E17">
+            <v>8192</v>
+          </cell>
+          <cell r="F17" t="str">
+            <v>No drive found</v>
+          </cell>
+          <cell r="G17">
+            <v>12.5</v>
+          </cell>
+          <cell r="H17" t="str">
+            <v>Needs check</v>
           </cell>
         </row>
       </sheetData>
@@ -801,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60981241-097C-4D7C-A446-9062E4E45EE4}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,6 +1299,28 @@
         <v>45079</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>45085</v>
+      </c>
+    </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
@@ -1051,93 +1482,104 @@
         <v>45079</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="2">
+        <v>45085</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="2">
-        <v>45079</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="2">
+        <v>45079</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>16</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C41" s="2">
         <v>45079</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B21">
-    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
       <formula>"INCOMPLETE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B21">
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
       <formula>"COMPLETE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:B36 B24:B31">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+  <conditionalFormatting sqref="B37:B38 B24:B32">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"COMPLETE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"INCOMPLETE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+  <conditionalFormatting sqref="B41">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"COMPLETE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"INCOMPLETE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"COMPLETE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"INCOMPLETE"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1151,7 +1593,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H40"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1666,7 @@
         <v>12.5</v>
       </c>
       <c r="H2" t="str">
-        <f>IF(COUNTIF(Components!B2:G2,"BAD")=0,"GOOD","BAD")</f>
+        <f>IF(COUNTIF(Components!B2:H2,"GOOD")=7,"GOOD","BAD")</f>
         <v>GOOD</v>
       </c>
     </row>
@@ -1258,483 +1700,483 @@
         <v>13.3</v>
       </c>
       <c r="H3" t="str">
-        <f>IF(COUNTIF(Components!B3:G3,"BAD")=0,"GOOD","BAD")</f>
+        <f>IF(COUNTIF(Components!B3:H3,"GOOD")=7,"GOOD","BAD")</f>
         <v>BAD</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" t="str">
         <f>[1]Inventory!A4</f>
-        <v>0</v>
-      </c>
-      <c r="B4">
+        <v>FJ9QLQ2</v>
+      </c>
+      <c r="B4" t="str">
         <f>[1]Inventory!B4</f>
-        <v>0</v>
-      </c>
-      <c r="C4">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C4" t="str">
         <f>[1]Inventory!C4</f>
-        <v>0</v>
-      </c>
-      <c r="D4">
+        <v>Latitude 5490</v>
+      </c>
+      <c r="D4" t="str">
         <f>[1]Inventory!D4</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E4">
         <f>[1]Inventory!E4</f>
-        <v>0</v>
-      </c>
-      <c r="F4">
+        <v>8192</v>
+      </c>
+      <c r="F4" t="str">
         <f>[1]Inventory!F4</f>
-        <v>0</v>
+        <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
       </c>
       <c r="G4">
         <f>[1]Inventory!G4</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H4" t="str">
-        <f>IF(COUNTIF(Components!B4:G4,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B4:H4,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" t="str">
         <f>[1]Inventory!A5</f>
-        <v>0</v>
-      </c>
-      <c r="B5">
+        <v>H4RFJR2</v>
+      </c>
+      <c r="B5" t="str">
         <f>[1]Inventory!B5</f>
-        <v>0</v>
-      </c>
-      <c r="C5">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C5" t="str">
         <f>[1]Inventory!C5</f>
-        <v>0</v>
-      </c>
-      <c r="D5">
+        <v>Latitude 5490</v>
+      </c>
+      <c r="D5" t="str">
         <f>[1]Inventory!D5</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E5">
         <f>[1]Inventory!E5</f>
-        <v>0</v>
-      </c>
-      <c r="F5">
+        <v>8192</v>
+      </c>
+      <c r="F5" t="str">
         <f>[1]Inventory!F5</f>
-        <v>0</v>
+        <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
       </c>
       <c r="G5">
         <f>[1]Inventory!G5</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H5" t="str">
-        <f>IF(COUNTIF(Components!B5:G5,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B5:H5,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" t="str">
         <f>[1]Inventory!A6</f>
-        <v>0</v>
-      </c>
-      <c r="B6">
+        <v>BBMJLQ2</v>
+      </c>
+      <c r="B6" t="str">
         <f>[1]Inventory!B6</f>
-        <v>0</v>
-      </c>
-      <c r="C6">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C6" t="str">
         <f>[1]Inventory!C6</f>
-        <v>0</v>
-      </c>
-      <c r="D6">
+        <v>Latitude 5490</v>
+      </c>
+      <c r="D6" t="str">
         <f>[1]Inventory!D6</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E6">
         <f>[1]Inventory!E6</f>
-        <v>0</v>
-      </c>
-      <c r="F6">
+        <v>8192</v>
+      </c>
+      <c r="F6" t="str">
         <f>[1]Inventory!F6</f>
-        <v>0</v>
+        <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
       </c>
       <c r="G6">
         <f>[1]Inventory!G6</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H6" t="str">
-        <f>IF(COUNTIF(Components!B6:G6,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B6:H6,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" t="str">
         <f>[1]Inventory!A7</f>
-        <v>0</v>
-      </c>
-      <c r="B7">
+        <v>HRQBQV2</v>
+      </c>
+      <c r="B7" t="str">
         <f>[1]Inventory!B7</f>
-        <v>0</v>
-      </c>
-      <c r="C7">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C7" t="str">
         <f>[1]Inventory!C7</f>
-        <v>0</v>
-      </c>
-      <c r="D7">
+        <v>Latitude 5490</v>
+      </c>
+      <c r="D7" t="str">
         <f>[1]Inventory!D7</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E7">
         <f>[1]Inventory!E7</f>
-        <v>0</v>
-      </c>
-      <c r="F7">
+        <v>8192</v>
+      </c>
+      <c r="F7" t="str">
         <f>[1]Inventory!F7</f>
-        <v>0</v>
+        <v>SK hynix SC401 SATA 256GB</v>
       </c>
       <c r="G7">
         <f>[1]Inventory!G7</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H7" t="str">
-        <f>IF(COUNTIF(Components!B7:G7,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B7:H7,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" t="str">
         <f>[1]Inventory!A8</f>
-        <v>0</v>
-      </c>
-      <c r="B8">
+        <v>C484M12</v>
+      </c>
+      <c r="B8" t="str">
         <f>[1]Inventory!B8</f>
-        <v>0</v>
-      </c>
-      <c r="C8">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C8" t="str">
         <f>[1]Inventory!C8</f>
-        <v>0</v>
-      </c>
-      <c r="D8">
+        <v>Latitude E6440</v>
+      </c>
+      <c r="D8" t="str">
         <f>[1]Inventory!D8</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-4310M CPU @ 2.70GHz</v>
       </c>
       <c r="E8">
         <f>[1]Inventory!E8</f>
-        <v>0</v>
-      </c>
-      <c r="F8">
+        <v>8192</v>
+      </c>
+      <c r="F8" t="str">
         <f>[1]Inventory!F8</f>
-        <v>0</v>
+        <v>LITEONIT LCS-180M6S-11 2.5 7mm 180GB</v>
       </c>
       <c r="G8">
         <f>[1]Inventory!G8</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H8" t="str">
-        <f>IF(COUNTIF(Components!B8:G8,"BAD")=0,"GOOD","BAD")</f>
+        <f>IF(COUNTIF(Components!B8:H8,"GOOD")=7,"GOOD","BAD")</f>
         <v>GOOD</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" t="str">
         <f>[1]Inventory!A9</f>
-        <v>0</v>
-      </c>
-      <c r="B9">
+        <v>29VM533</v>
+      </c>
+      <c r="B9" t="str">
         <f>[1]Inventory!B9</f>
-        <v>0</v>
-      </c>
-      <c r="C9">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C9" t="str">
         <f>[1]Inventory!C9</f>
-        <v>0</v>
-      </c>
-      <c r="D9">
+        <v>Latitude 5400</v>
+      </c>
+      <c r="D9" t="str">
         <f>[1]Inventory!D9</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8265U CPU @ 1.60GHz</v>
       </c>
       <c r="E9">
         <f>[1]Inventory!E9</f>
-        <v>0</v>
-      </c>
-      <c r="F9">
+        <v>8192</v>
+      </c>
+      <c r="F9" t="str">
         <f>[1]Inventory!F9</f>
-        <v>0</v>
+        <v>PM991 NVMe Samsung 256GB</v>
       </c>
       <c r="G9">
         <f>[1]Inventory!G9</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H9" t="str">
-        <f>IF(COUNTIF(Components!B9:G9,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B9:H9,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" t="str">
         <f>[1]Inventory!A10</f>
-        <v>0</v>
-      </c>
-      <c r="B10">
+        <v>5DRF3M2</v>
+      </c>
+      <c r="B10" t="str">
         <f>[1]Inventory!B10</f>
-        <v>0</v>
-      </c>
-      <c r="C10">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C10" t="str">
         <f>[1]Inventory!C10</f>
-        <v>0</v>
-      </c>
-      <c r="D10">
+        <v>Latitude 5480</v>
+      </c>
+      <c r="D10" t="str">
         <f>[1]Inventory!D10</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-7200U CPU @ 2.50GHz</v>
       </c>
       <c r="E10">
         <f>[1]Inventory!E10</f>
-        <v>0</v>
-      </c>
-      <c r="F10">
+        <v>16384</v>
+      </c>
+      <c r="F10" t="str">
         <f>[1]Inventory!F10</f>
-        <v>0</v>
+        <v>SK hynix SC308 SATA 128GB</v>
       </c>
       <c r="G10">
         <f>[1]Inventory!G10</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H10" t="str">
-        <f>IF(COUNTIF(Components!B10:G10,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B10:H10,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" t="str">
         <f>[1]Inventory!A11</f>
-        <v>0</v>
-      </c>
-      <c r="B11">
+        <v>CB8NQQ2</v>
+      </c>
+      <c r="B11" t="str">
         <f>[1]Inventory!B11</f>
-        <v>0</v>
-      </c>
-      <c r="C11">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C11" t="str">
         <f>[1]Inventory!C11</f>
-        <v>0</v>
-      </c>
-      <c r="D11">
+        <v>Latitude 5490</v>
+      </c>
+      <c r="D11" t="str">
         <f>[1]Inventory!D11</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E11">
         <f>[1]Inventory!E11</f>
-        <v>0</v>
-      </c>
-      <c r="F11">
+        <v>8192</v>
+      </c>
+      <c r="F11" t="str">
         <f>[1]Inventory!F11</f>
-        <v>0</v>
+        <v>SK hynix SC311 SATA 256GB</v>
       </c>
       <c r="G11">
         <f>[1]Inventory!G11</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H11" t="str">
-        <f>IF(COUNTIF(Components!B11:G11,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B11:H11,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" t="str">
         <f>[1]Inventory!A12</f>
-        <v>0</v>
-      </c>
-      <c r="B12">
+        <v>7KW9QQ2</v>
+      </c>
+      <c r="B12" t="str">
         <f>[1]Inventory!B12</f>
-        <v>0</v>
-      </c>
-      <c r="C12">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C12" t="str">
         <f>[1]Inventory!C12</f>
-        <v>0</v>
-      </c>
-      <c r="D12">
+        <v>Latitude 5490</v>
+      </c>
+      <c r="D12" t="str">
         <f>[1]Inventory!D12</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E12">
         <f>[1]Inventory!E12</f>
-        <v>0</v>
-      </c>
-      <c r="F12">
+        <v>8192</v>
+      </c>
+      <c r="F12" t="str">
         <f>[1]Inventory!F12</f>
-        <v>0</v>
+        <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
       </c>
       <c r="G12">
         <f>[1]Inventory!G12</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H12" t="str">
-        <f>IF(COUNTIF(Components!B12:G12,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B12:H12,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" t="str">
         <f>[1]Inventory!A13</f>
-        <v>0</v>
-      </c>
-      <c r="B13">
+        <v>38MTNN2</v>
+      </c>
+      <c r="B13" t="str">
         <f>[1]Inventory!B13</f>
-        <v>0</v>
-      </c>
-      <c r="C13">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C13" t="str">
         <f>[1]Inventory!C13</f>
-        <v>0</v>
-      </c>
-      <c r="D13">
+        <v>Latitude 5580</v>
+      </c>
+      <c r="D13" t="str">
         <f>[1]Inventory!D13</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-7300U CPU @ 2.60GHz</v>
       </c>
       <c r="E13">
         <f>[1]Inventory!E13</f>
-        <v>0</v>
-      </c>
-      <c r="F13">
+        <v>16384</v>
+      </c>
+      <c r="F13" t="str">
         <f>[1]Inventory!F13</f>
-        <v>0</v>
+        <v>SK hynix SC401 SATA 256GB</v>
       </c>
       <c r="G13">
         <f>[1]Inventory!G13</f>
-        <v>0</v>
+        <v>15.6</v>
       </c>
       <c r="H13" t="str">
-        <f>IF(COUNTIF(Components!B13:G13,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B13:H13,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" t="str">
         <f>[1]Inventory!A14</f>
-        <v>0</v>
-      </c>
-      <c r="B14">
+        <v>CVJJMQ2</v>
+      </c>
+      <c r="B14" t="str">
         <f>[1]Inventory!B14</f>
-        <v>0</v>
-      </c>
-      <c r="C14">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C14" t="str">
         <f>[1]Inventory!C14</f>
-        <v>0</v>
-      </c>
-      <c r="D14">
+        <v>Latitude 5590</v>
+      </c>
+      <c r="D14" t="str">
         <f>[1]Inventory!D14</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E14">
         <f>[1]Inventory!E14</f>
-        <v>0</v>
-      </c>
-      <c r="F14">
+        <v>8192</v>
+      </c>
+      <c r="F14" t="str">
         <f>[1]Inventory!F14</f>
-        <v>0</v>
+        <v>WDC WD5000LPLX-75ZNTT0</v>
       </c>
       <c r="G14">
         <f>[1]Inventory!G14</f>
-        <v>0</v>
+        <v>15.6</v>
       </c>
       <c r="H14" t="str">
-        <f>IF(COUNTIF(Components!B14:G14,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B14:H14,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" t="str">
         <f>[1]Inventory!A15</f>
-        <v>0</v>
-      </c>
-      <c r="B15">
+        <v>6L6RMQ2</v>
+      </c>
+      <c r="B15" t="str">
         <f>[1]Inventory!B15</f>
-        <v>0</v>
-      </c>
-      <c r="C15">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C15" t="str">
         <f>[1]Inventory!C15</f>
-        <v>0</v>
-      </c>
-      <c r="D15">
+        <v>Latitude 5490</v>
+      </c>
+      <c r="D15" t="str">
         <f>[1]Inventory!D15</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E15">
         <f>[1]Inventory!E15</f>
-        <v>0</v>
-      </c>
-      <c r="F15">
+        <v>8192</v>
+      </c>
+      <c r="F15" t="str">
         <f>[1]Inventory!F15</f>
-        <v>0</v>
+        <v>Micron 1100 SATA 256GB</v>
       </c>
       <c r="G15">
         <f>[1]Inventory!G15</f>
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="H15" t="str">
-        <f>IF(COUNTIF(Components!B15:G15,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B15:H15,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" t="str">
         <f>[1]Inventory!A16</f>
-        <v>0</v>
-      </c>
-      <c r="B16">
+        <v>H0J05S2</v>
+      </c>
+      <c r="B16" t="str">
         <f>[1]Inventory!B16</f>
-        <v>0</v>
-      </c>
-      <c r="C16">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C16" t="str">
         <f>[1]Inventory!C16</f>
-        <v>0</v>
-      </c>
-      <c r="D16">
+        <v>Latitude 5490</v>
+      </c>
+      <c r="D16" t="str">
         <f>[1]Inventory!D16</f>
-        <v>0</v>
+        <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E16">
         <f>[1]Inventory!E16</f>
-        <v>0</v>
-      </c>
-      <c r="F16">
+        <v>8192</v>
+      </c>
+      <c r="F16" t="str">
         <f>[1]Inventory!F16</f>
-        <v>0</v>
+        <v>No drive found</v>
       </c>
       <c r="G16">
         <f>[1]Inventory!G16</f>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="H16" t="str">
-        <f>IF(COUNTIF(Components!B16:G16,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B16:H16,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" t="str">
         <f>[1]Inventory!A17</f>
-        <v>0</v>
-      </c>
-      <c r="B17">
+        <v>JR64Q32</v>
+      </c>
+      <c r="B17" t="str">
         <f>[1]Inventory!B17</f>
-        <v>0</v>
-      </c>
-      <c r="C17">
+        <v>Dell Inc.</v>
+      </c>
+      <c r="C17" t="str">
         <f>[1]Inventory!C17</f>
-        <v>0</v>
-      </c>
-      <c r="D17">
+        <v>Latitude E7250</v>
+      </c>
+      <c r="D17" t="str">
         <f>[1]Inventory!D17</f>
-        <v>0</v>
+        <v>No CPU found</v>
       </c>
       <c r="E17">
         <f>[1]Inventory!E17</f>
-        <v>0</v>
-      </c>
-      <c r="F17">
+        <v>8192</v>
+      </c>
+      <c r="F17" t="str">
         <f>[1]Inventory!F17</f>
-        <v>0</v>
+        <v>No drive found</v>
       </c>
       <c r="G17">
         <f>[1]Inventory!G17</f>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="H17" t="str">
-        <f>IF(COUNTIF(Components!B17:G17,"BAD")=0,"GOOD","BAD")</f>
+        <f>IF(COUNTIF(Components!B17:H17,"GOOD")=7,"GOOD","BAD")</f>
         <v>GOOD</v>
       </c>
     </row>
@@ -1768,8 +2210,8 @@
         <v>0</v>
       </c>
       <c r="H18" t="str">
-        <f>IF(COUNTIF(Components!B18:G18,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B18:H18,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1802,8 +2244,8 @@
         <v>0</v>
       </c>
       <c r="H19" t="str">
-        <f>IF(COUNTIF(Components!B19:G19,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B19:H19,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1836,8 +2278,8 @@
         <v>0</v>
       </c>
       <c r="H20" t="str">
-        <f>IF(COUNTIF(Components!B20:G20,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B20:H20,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1870,8 +2312,8 @@
         <v>0</v>
       </c>
       <c r="H21" t="str">
-        <f>IF(COUNTIF(Components!B21:G21,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B21:H21,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1904,8 +2346,8 @@
         <v>0</v>
       </c>
       <c r="H22" t="str">
-        <f>IF(COUNTIF(Components!B22:G22,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B22:H22,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1938,8 +2380,8 @@
         <v>0</v>
       </c>
       <c r="H23" t="str">
-        <f>IF(COUNTIF(Components!B23:G23,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B23:H23,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1972,8 +2414,8 @@
         <v>0</v>
       </c>
       <c r="H24" t="str">
-        <f>IF(COUNTIF(Components!B24:G24,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B24:H24,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2006,8 +2448,8 @@
         <v>0</v>
       </c>
       <c r="H25" t="str">
-        <f>IF(COUNTIF(Components!B25:G25,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B25:H25,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2040,8 +2482,8 @@
         <v>0</v>
       </c>
       <c r="H26" t="str">
-        <f>IF(COUNTIF(Components!B26:G26,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B26:H26,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2074,8 +2516,8 @@
         <v>0</v>
       </c>
       <c r="H27" t="str">
-        <f>IF(COUNTIF(Components!B27:G27,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B27:H27,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2108,8 +2550,8 @@
         <v>0</v>
       </c>
       <c r="H28" t="str">
-        <f>IF(COUNTIF(Components!B28:G28,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B28:H28,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2142,8 +2584,8 @@
         <v>0</v>
       </c>
       <c r="H29" t="str">
-        <f>IF(COUNTIF(Components!B29:G29,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B29:H29,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2176,8 +2618,8 @@
         <v>0</v>
       </c>
       <c r="H30" t="str">
-        <f>IF(COUNTIF(Components!B30:G30,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B30:H30,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2210,8 +2652,8 @@
         <v>0</v>
       </c>
       <c r="H31" t="str">
-        <f>IF(COUNTIF(Components!B31:G31,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B31:H31,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2244,8 +2686,8 @@
         <v>0</v>
       </c>
       <c r="H32" t="str">
-        <f>IF(COUNTIF(Components!B32:G32,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B32:H32,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2278,8 +2720,8 @@
         <v>0</v>
       </c>
       <c r="H33" t="str">
-        <f>IF(COUNTIF(Components!B33:G33,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B33:H33,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2312,8 +2754,8 @@
         <v>0</v>
       </c>
       <c r="H34" t="str">
-        <f>IF(COUNTIF(Components!B34:G34,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B34:H34,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2346,8 +2788,8 @@
         <v>0</v>
       </c>
       <c r="H35" t="str">
-        <f>IF(COUNTIF(Components!B35:G35,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B35:H35,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2380,8 +2822,8 @@
         <v>0</v>
       </c>
       <c r="H36" t="str">
-        <f>IF(COUNTIF(Components!B36:G36,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B36:H36,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2414,8 +2856,8 @@
         <v>0</v>
       </c>
       <c r="H37" t="str">
-        <f>IF(COUNTIF(Components!B37:G37,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B37:H37,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2448,8 +2890,8 @@
         <v>0</v>
       </c>
       <c r="H38" t="str">
-        <f>IF(COUNTIF(Components!B38:G38,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B38:H38,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2482,8 +2924,8 @@
         <v>0</v>
       </c>
       <c r="H39" t="str">
-        <f>IF(COUNTIF(Components!B39:G39,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B39:H39,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2516,17 +2958,17 @@
         <v>0</v>
       </c>
       <c r="H40" t="str">
-        <f>IF(COUNTIF(Components!B40:G40,"BAD")=0,"GOOD","BAD")</f>
-        <v>GOOD</v>
+        <f>IF(COUNTIF(Components!B40:H40,"GOOD")=7,"GOOD","BAD")</f>
+        <v>BAD</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H40">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"GOOD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"BAD"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
-      <formula>"GOOD"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2535,19 +2977,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72495FFC-BCFC-452F-9FB3-17F398D4E024}">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="67.5703125" customWidth="1"/>
+    <col min="9" max="9" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
         <f>Inventory!A1</f>
         <v>Serial</v>
@@ -2571,10 +3013,13 @@
         <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>Inventory!A2</f>
         <v>9442Q32</v>
@@ -2597,8 +3042,11 @@
       <c r="G2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>Inventory!A3</f>
         <v>J703QV2</v>
@@ -2619,734 +3067,1514 @@
         <v>39</v>
       </c>
       <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>Inventory!A4</f>
+        <v>FJ9QLQ2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
         <v>40</v>
       </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>Inventory!A4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="str">
+        <f>[1]Inventory!H4</f>
+        <v>No battery; bad trackpad</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
         <f>Inventory!A5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <v>H4RFJR2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="str">
+        <f>[1]Inventory!H5</f>
+        <v>Bad battery; random shutdowns; no esc key</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
         <f>Inventory!A6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+        <v>BBMJLQ2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="str">
+        <f>[1]Inventory!H6</f>
+        <v>No battery; no hdd</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
         <f>Inventory!A7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+        <v>HRQBQV2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="str">
+        <f>[1]Inventory!H7</f>
+        <v>No battery; USB-C cosmetic damage</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
         <f>Inventory!A8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+        <v>C484M12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="str">
+        <f>[1]Inventory!H8</f>
+        <v>Needs cleaning and check</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
         <f>Inventory!A9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+        <v>29VM533</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="str">
+        <f>[1]Inventory!H9</f>
+        <v>No battery; bad screen</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
         <f>Inventory!A10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+        <v>5DRF3M2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="str">
+        <f>[1]Inventory!H10</f>
+        <v>No battery; bad hdd</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
         <f>Inventory!A11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
+        <v>CB8NQQ2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="str">
+        <f>[1]Inventory!H11</f>
+        <v>No battery; no ram; bad keyboard</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
         <f>Inventory!A12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
+        <v>7KW9QQ2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" t="str">
+        <f>[1]Inventory!H12</f>
+        <v>No battery; bad keyboard; front cover bulge; bad drivers</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
         <f>Inventory!A13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
+        <v>38MTNN2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" t="str">
+        <f>[1]Inventory!H13</f>
+        <v>No battery; no ram; bad ethernet; ALIAS VMNB0128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
         <f>Inventory!A14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
+        <v>CVJJMQ2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" t="str">
+        <f>[1]Inventory!H14</f>
+        <v>No battery; ALIAS VMNB0131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
         <f>Inventory!A15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
+        <v>6L6RMQ2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" t="str">
+        <f>[1]Inventory!H15</f>
+        <v>No battery; no j key or joystick; no trackpad buttons</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
         <f>Inventory!A16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
+        <v>H0J05S2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" t="str">
+        <f>[1]Inventory!H16</f>
+        <v>Don't even bother</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
         <f>Inventory!A17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>JR64Q32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" t="str">
+        <f>[1]Inventory!H17</f>
+        <v>Needs check</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>Inventory!A18</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f>[1]Inventory!H18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>Inventory!A19</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f>[1]Inventory!H19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>Inventory!A20</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f>[1]Inventory!H20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>Inventory!A21</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f>[1]Inventory!H21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>Inventory!A22</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f>[1]Inventory!H22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>Inventory!A23</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f>[1]Inventory!H23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>Inventory!A24</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f>[1]Inventory!H24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>Inventory!A25</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f>[1]Inventory!H25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>Inventory!A26</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f>[1]Inventory!H26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>Inventory!A27</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f>[1]Inventory!H27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>Inventory!A28</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f>[1]Inventory!H28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>Inventory!A29</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f>[1]Inventory!H29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>Inventory!A30</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f>[1]Inventory!H30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>Inventory!A31</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <f>[1]Inventory!H31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>Inventory!A32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <f>[1]Inventory!H32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>Inventory!A33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f>[1]Inventory!H33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>Inventory!A34</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <f>[1]Inventory!H34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>Inventory!A35</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <f>[1]Inventory!H35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>Inventory!A36</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <f>[1]Inventory!H36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>Inventory!A37</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <f>[1]Inventory!H37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>Inventory!A38</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <f>[1]Inventory!H38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>Inventory!A39</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <f>[1]Inventory!H39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>Inventory!A40</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <f>[1]Inventory!H40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>Inventory!A41</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <f>[1]Inventory!H41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>Inventory!A42</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <f>[1]Inventory!H42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>Inventory!A43</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <f>[1]Inventory!H43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>Inventory!A44</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <f>[1]Inventory!H44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>Inventory!A45</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <f>[1]Inventory!H45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>Inventory!A46</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <f>[1]Inventory!H46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>Inventory!A47</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <f>[1]Inventory!H47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <f>Inventory!A48</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <f>[1]Inventory!H48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <f>Inventory!A49</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <f>[1]Inventory!H49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>Inventory!A50</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <f>[1]Inventory!H50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <f>Inventory!A51</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <f>[1]Inventory!H51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <f>Inventory!A52</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <f>[1]Inventory!H52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <f>Inventory!A53</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <f>[1]Inventory!H53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <f>Inventory!A54</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <f>[1]Inventory!H54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <f>Inventory!A55</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <f>[1]Inventory!H55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>Inventory!A56</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <f>[1]Inventory!H56</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <f>Inventory!A57</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <f>[1]Inventory!H57</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <f>Inventory!A58</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <f>[1]Inventory!H58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <f>Inventory!A59</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <f>[1]Inventory!H59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <f>Inventory!A60</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <f>[1]Inventory!H60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <f>Inventory!A61</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <f>[1]Inventory!H61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <f>Inventory!A62</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <f>[1]Inventory!H62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <f>Inventory!A63</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <f>[1]Inventory!H63</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <f>Inventory!A64</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <f>[1]Inventory!H64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <f>Inventory!A65</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <f>[1]Inventory!H65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <f>Inventory!A66</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <f>[1]Inventory!H66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <f>Inventory!A67</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <f>[1]Inventory!H67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <f>Inventory!A68</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <f>[1]Inventory!H68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <f>Inventory!A69</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <f>[1]Inventory!H69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <f>Inventory!A70</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <f>[1]Inventory!H70</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <f>Inventory!A71</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <f>[1]Inventory!H71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <f>Inventory!A72</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <f>[1]Inventory!H72</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <f>Inventory!A73</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <f>[1]Inventory!H73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <f>Inventory!A74</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <f>[1]Inventory!H74</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <f>Inventory!A75</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I75">
+        <f>[1]Inventory!H75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <f>Inventory!A76</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I76">
+        <f>[1]Inventory!H76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <f>Inventory!A77</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <f>[1]Inventory!H77</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <f>Inventory!A78</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <f>[1]Inventory!H78</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <f>Inventory!A79</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <f>[1]Inventory!H79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <f>Inventory!A80</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <f>[1]Inventory!H80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <f>Inventory!A81</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <f>[1]Inventory!H81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <f>Inventory!A82</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <f>[1]Inventory!H82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <f>Inventory!A83</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <f>[1]Inventory!H83</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <f>Inventory!A84</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <f>[1]Inventory!H84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <f>Inventory!A85</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <f>[1]Inventory!H85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <f>Inventory!A86</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <f>[1]Inventory!H86</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <f>Inventory!A87</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <f>[1]Inventory!H87</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <f>Inventory!A88</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <f>[1]Inventory!H88</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <f>Inventory!A89</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <f>[1]Inventory!H89</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <f>Inventory!A90</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <f>[1]Inventory!H90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <f>Inventory!A91</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I91">
+        <f>[1]Inventory!H91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <f>Inventory!A92</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I92">
+        <f>[1]Inventory!H92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <f>Inventory!A93</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I93">
+        <f>[1]Inventory!H93</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <f>Inventory!A94</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I94">
+        <f>[1]Inventory!H94</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <f>Inventory!A95</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I95">
+        <f>[1]Inventory!H95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <f>Inventory!A96</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I96">
+        <f>[1]Inventory!H96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <f>Inventory!A97</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I97">
+        <f>[1]Inventory!H97</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <f>Inventory!A98</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I98">
+        <f>[1]Inventory!H98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <f>Inventory!A99</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I99">
+        <f>[1]Inventory!H99</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <f>Inventory!A100</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I100">
+        <f>[1]Inventory!H100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <f>Inventory!A101</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I101">
+        <f>[1]Inventory!H101</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
         <f>Inventory!A102</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I102">
+        <f>[1]Inventory!H102</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
         <f>Inventory!A103</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I103">
+        <f>[1]Inventory!H103</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104">
         <f>Inventory!A104</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I104">
+        <f>[1]Inventory!H104</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105">
         <f>Inventory!A105</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I105">
+        <f>[1]Inventory!H105</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106">
         <f>Inventory!A106</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I106">
+        <f>[1]Inventory!H106</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
         <f>Inventory!A107</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I107">
+        <f>[1]Inventory!H107</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108">
         <f>Inventory!A108</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I108">
+        <f>[1]Inventory!H108</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109">
         <f>Inventory!A109</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I109">
+        <f>[1]Inventory!H109</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110">
         <f>Inventory!A110</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I110">
+        <f>[1]Inventory!H110</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111">
         <f>Inventory!A111</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I111">
+        <f>[1]Inventory!H111</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112">
         <f>Inventory!A112</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I112">
+        <f>[1]Inventory!H112</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113">
         <f>Inventory!A113</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I113">
+        <f>[1]Inventory!H113</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114">
         <f>Inventory!A114</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I114">
+        <f>[1]Inventory!H114</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115">
         <f>Inventory!A115</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I115">
+        <f>[1]Inventory!H115</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
         <f>Inventory!A116</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I116">
+        <f>[1]Inventory!H116</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117">
         <f>Inventory!A117</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I117">
+        <f>[1]Inventory!H117</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118">
         <f>Inventory!A118</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I118">
+        <f>[1]Inventory!H118</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
         <f>Inventory!A119</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I119">
+        <f>[1]Inventory!H119</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
         <f>Inventory!A120</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I120">
+        <f>[1]Inventory!H120</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
         <f>Inventory!A121</f>
         <v>0</v>
       </c>
+      <c r="I121">
+        <f>[1]Inventory!H121</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:G271 H3">
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+  <conditionalFormatting sqref="I3">
+    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
+      <formula>"GOOD"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="17" operator="equal">
       <formula>"BAD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"GOOD"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"BAD"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G271 H3">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="B1:H1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"NONE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"GOOD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"BAD"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed "No HDD detected" issue
Had variable "driveID" undeclared from previous push
</commit_message>
<xml_diff>
--- a/Progress Tracker.xlsx
+++ b/Progress Tracker.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="290" documentId="8_{57302A05-458C-48CC-8B27-F26F6D4EC990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F1BF58F-030B-4C42-86BB-60726C528F3E}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FA77BBBF-EB64-490E-8DDD-6B84D43932A0}"/>
   </bookViews>
   <sheets>
     <sheet name="App Dev Log" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1212,18 +1212,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60981241-097C-4D7C-A446-9062E4E45EE4}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1234,17 +1234,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>45076</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>45079</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>45079</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>45076</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>45079</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>45084</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1321,12 +1321,12 @@
         <v>45085</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>45082</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>45079</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1367,34 +1367,34 @@
         <v>45082</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>45076</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>45077</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>45077</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>45076</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>45077</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>45079</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>45076</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>45079</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>45085</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -1509,12 +1509,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>45079</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1592,77 +1592,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D6CEEC-0B88-42F6-AACF-13F799424260}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+    <col min="4" max="4" width="41.26953125" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" customWidth="1"/>
+    <col min="6" max="6" width="33.81640625" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
-        <f>[1]Inventory!A1</f>
+        <f ca="1">[1]Inventory!A1</f>
         <v>Serial</v>
       </c>
       <c r="B1" s="1" t="str">
-        <f>[1]Inventory!B1</f>
+        <f ca="1">[1]Inventory!B1</f>
         <v>Manufacturer</v>
       </c>
       <c r="C1" s="1" t="str">
-        <f>[1]Inventory!C1</f>
+        <f ca="1">[1]Inventory!C1</f>
         <v>Model</v>
       </c>
       <c r="D1" s="1" t="str">
-        <f>[1]Inventory!D1</f>
+        <f ca="1">[1]Inventory!D1</f>
         <v>CPU</v>
       </c>
       <c r="E1" s="1" t="str">
-        <f>[1]Inventory!E1</f>
+        <f ca="1">[1]Inventory!E1</f>
         <v>Memory</v>
       </c>
       <c r="F1" s="1" t="str">
-        <f>[1]Inventory!F1</f>
+        <f ca="1">[1]Inventory!F1</f>
         <v>HDD</v>
       </c>
       <c r="G1" s="1" t="str">
-        <f>[1]Inventory!G1</f>
+        <f ca="1">[1]Inventory!G1</f>
         <v>Screen Size</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
-        <f>[1]Inventory!A2</f>
+        <f ca="1">[1]Inventory!A2</f>
         <v>9442Q32</v>
       </c>
       <c r="B2" t="str">
-        <f>[1]Inventory!B2</f>
+        <f ca="1">[1]Inventory!B2</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C2" t="str">
-        <f>[1]Inventory!C2</f>
+        <f ca="1">[1]Inventory!C2</f>
         <v>Latitude E7250</v>
       </c>
       <c r="D2" t="str">
-        <f>[1]Inventory!D2</f>
+        <f ca="1">[1]Inventory!D2</f>
         <v>Intel(R) Core(TM) i7-5600U CPU @ 2.60GHz</v>
       </c>
       <c r="E2">
-        <f>[1]Inventory!E2</f>
+        <f ca="1">[1]Inventory!E2</f>
         <v>8192</v>
       </c>
       <c r="F2" t="str">
-        <f>[1]Inventory!F2</f>
+        <f ca="1">[1]Inventory!F2</f>
         <v>SAMSUNG SSD PM851 mSATA 256GB</v>
       </c>
       <c r="G2">
-        <f>[1]Inventory!G2</f>
+        <f ca="1">[1]Inventory!G2</f>
         <v>12.5</v>
       </c>
       <c r="H2" t="str">
@@ -1670,33 +1670,33 @@
         <v>GOOD</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
-        <f>[1]Inventory!A3</f>
+        <f ca="1">[1]Inventory!A3</f>
         <v>J703QV2</v>
       </c>
       <c r="B3" t="str">
-        <f>[1]Inventory!B3</f>
+        <f ca="1">[1]Inventory!B3</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C3" t="str">
-        <f>[1]Inventory!C3</f>
+        <f ca="1">[1]Inventory!C3</f>
         <v>Latitude 5490</v>
       </c>
       <c r="D3" t="str">
-        <f>[1]Inventory!D3</f>
+        <f ca="1">[1]Inventory!D3</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E3">
-        <f>[1]Inventory!E3</f>
+        <f ca="1">[1]Inventory!E3</f>
         <v>8192</v>
       </c>
       <c r="F3" t="str">
-        <f>[1]Inventory!F3</f>
+        <f ca="1">[1]Inventory!F3</f>
         <v>SanDisk X600 M.2 2280 SATA 256GB</v>
       </c>
       <c r="G3">
-        <f>[1]Inventory!G3</f>
+        <f ca="1">[1]Inventory!G3</f>
         <v>13.3</v>
       </c>
       <c r="H3" t="str">
@@ -1704,33 +1704,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
-        <f>[1]Inventory!A4</f>
+        <f ca="1">[1]Inventory!A4</f>
         <v>FJ9QLQ2</v>
       </c>
       <c r="B4" t="str">
-        <f>[1]Inventory!B4</f>
+        <f ca="1">[1]Inventory!B4</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C4" t="str">
-        <f>[1]Inventory!C4</f>
+        <f ca="1">[1]Inventory!C4</f>
         <v>Latitude 5490</v>
       </c>
       <c r="D4" t="str">
-        <f>[1]Inventory!D4</f>
+        <f ca="1">[1]Inventory!D4</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E4">
-        <f>[1]Inventory!E4</f>
+        <f ca="1">[1]Inventory!E4</f>
         <v>8192</v>
       </c>
       <c r="F4" t="str">
-        <f>[1]Inventory!F4</f>
+        <f ca="1">[1]Inventory!F4</f>
         <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
       </c>
       <c r="G4">
-        <f>[1]Inventory!G4</f>
+        <f ca="1">[1]Inventory!G4</f>
         <v>13.3</v>
       </c>
       <c r="H4" t="str">
@@ -1738,33 +1738,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
-        <f>[1]Inventory!A5</f>
+        <f ca="1">[1]Inventory!A5</f>
         <v>H4RFJR2</v>
       </c>
       <c r="B5" t="str">
-        <f>[1]Inventory!B5</f>
+        <f ca="1">[1]Inventory!B5</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C5" t="str">
-        <f>[1]Inventory!C5</f>
+        <f ca="1">[1]Inventory!C5</f>
         <v>Latitude 5490</v>
       </c>
       <c r="D5" t="str">
-        <f>[1]Inventory!D5</f>
+        <f ca="1">[1]Inventory!D5</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E5">
-        <f>[1]Inventory!E5</f>
+        <f ca="1">[1]Inventory!E5</f>
         <v>8192</v>
       </c>
       <c r="F5" t="str">
-        <f>[1]Inventory!F5</f>
+        <f ca="1">[1]Inventory!F5</f>
         <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
       </c>
       <c r="G5">
-        <f>[1]Inventory!G5</f>
+        <f ca="1">[1]Inventory!G5</f>
         <v>13.3</v>
       </c>
       <c r="H5" t="str">
@@ -1772,33 +1772,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
-        <f>[1]Inventory!A6</f>
+        <f ca="1">[1]Inventory!A6</f>
         <v>BBMJLQ2</v>
       </c>
       <c r="B6" t="str">
-        <f>[1]Inventory!B6</f>
+        <f ca="1">[1]Inventory!B6</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C6" t="str">
-        <f>[1]Inventory!C6</f>
+        <f ca="1">[1]Inventory!C6</f>
         <v>Latitude 5490</v>
       </c>
       <c r="D6" t="str">
-        <f>[1]Inventory!D6</f>
+        <f ca="1">[1]Inventory!D6</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E6">
-        <f>[1]Inventory!E6</f>
+        <f ca="1">[1]Inventory!E6</f>
         <v>8192</v>
       </c>
       <c r="F6" t="str">
-        <f>[1]Inventory!F6</f>
+        <f ca="1">[1]Inventory!F6</f>
         <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
       </c>
       <c r="G6">
-        <f>[1]Inventory!G6</f>
+        <f ca="1">[1]Inventory!G6</f>
         <v>13.3</v>
       </c>
       <c r="H6" t="str">
@@ -1806,33 +1806,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
-        <f>[1]Inventory!A7</f>
+        <f ca="1">[1]Inventory!A7</f>
         <v>HRQBQV2</v>
       </c>
       <c r="B7" t="str">
-        <f>[1]Inventory!B7</f>
+        <f ca="1">[1]Inventory!B7</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C7" t="str">
-        <f>[1]Inventory!C7</f>
+        <f ca="1">[1]Inventory!C7</f>
         <v>Latitude 5490</v>
       </c>
       <c r="D7" t="str">
-        <f>[1]Inventory!D7</f>
+        <f ca="1">[1]Inventory!D7</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E7">
-        <f>[1]Inventory!E7</f>
+        <f ca="1">[1]Inventory!E7</f>
         <v>8192</v>
       </c>
       <c r="F7" t="str">
-        <f>[1]Inventory!F7</f>
+        <f ca="1">[1]Inventory!F7</f>
         <v>SK hynix SC401 SATA 256GB</v>
       </c>
       <c r="G7">
-        <f>[1]Inventory!G7</f>
+        <f ca="1">[1]Inventory!G7</f>
         <v>13.3</v>
       </c>
       <c r="H7" t="str">
@@ -1840,33 +1840,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
-        <f>[1]Inventory!A8</f>
+        <f ca="1">[1]Inventory!A8</f>
         <v>C484M12</v>
       </c>
       <c r="B8" t="str">
-        <f>[1]Inventory!B8</f>
+        <f ca="1">[1]Inventory!B8</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C8" t="str">
-        <f>[1]Inventory!C8</f>
+        <f ca="1">[1]Inventory!C8</f>
         <v>Latitude E6440</v>
       </c>
       <c r="D8" t="str">
-        <f>[1]Inventory!D8</f>
+        <f ca="1">[1]Inventory!D8</f>
         <v>Intel(R) Core(TM) i5-4310M CPU @ 2.70GHz</v>
       </c>
       <c r="E8">
-        <f>[1]Inventory!E8</f>
+        <f ca="1">[1]Inventory!E8</f>
         <v>8192</v>
       </c>
       <c r="F8" t="str">
-        <f>[1]Inventory!F8</f>
+        <f ca="1">[1]Inventory!F8</f>
         <v>LITEONIT LCS-180M6S-11 2.5 7mm 180GB</v>
       </c>
       <c r="G8">
-        <f>[1]Inventory!G8</f>
+        <f ca="1">[1]Inventory!G8</f>
         <v>13.3</v>
       </c>
       <c r="H8" t="str">
@@ -1874,33 +1874,33 @@
         <v>GOOD</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
-        <f>[1]Inventory!A9</f>
+        <f ca="1">[1]Inventory!A9</f>
         <v>29VM533</v>
       </c>
       <c r="B9" t="str">
-        <f>[1]Inventory!B9</f>
+        <f ca="1">[1]Inventory!B9</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C9" t="str">
-        <f>[1]Inventory!C9</f>
+        <f ca="1">[1]Inventory!C9</f>
         <v>Latitude 5400</v>
       </c>
       <c r="D9" t="str">
-        <f>[1]Inventory!D9</f>
+        <f ca="1">[1]Inventory!D9</f>
         <v>Intel(R) Core(TM) i5-8265U CPU @ 1.60GHz</v>
       </c>
       <c r="E9">
-        <f>[1]Inventory!E9</f>
+        <f ca="1">[1]Inventory!E9</f>
         <v>8192</v>
       </c>
       <c r="F9" t="str">
-        <f>[1]Inventory!F9</f>
+        <f ca="1">[1]Inventory!F9</f>
         <v>PM991 NVMe Samsung 256GB</v>
       </c>
       <c r="G9">
-        <f>[1]Inventory!G9</f>
+        <f ca="1">[1]Inventory!G9</f>
         <v>13.3</v>
       </c>
       <c r="H9" t="str">
@@ -1908,33 +1908,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
-        <f>[1]Inventory!A10</f>
+        <f ca="1">[1]Inventory!A10</f>
         <v>5DRF3M2</v>
       </c>
       <c r="B10" t="str">
-        <f>[1]Inventory!B10</f>
+        <f ca="1">[1]Inventory!B10</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C10" t="str">
-        <f>[1]Inventory!C10</f>
+        <f ca="1">[1]Inventory!C10</f>
         <v>Latitude 5480</v>
       </c>
       <c r="D10" t="str">
-        <f>[1]Inventory!D10</f>
+        <f ca="1">[1]Inventory!D10</f>
         <v>Intel(R) Core(TM) i5-7200U CPU @ 2.50GHz</v>
       </c>
       <c r="E10">
-        <f>[1]Inventory!E10</f>
+        <f ca="1">[1]Inventory!E10</f>
         <v>16384</v>
       </c>
       <c r="F10" t="str">
-        <f>[1]Inventory!F10</f>
+        <f ca="1">[1]Inventory!F10</f>
         <v>SK hynix SC308 SATA 128GB</v>
       </c>
       <c r="G10">
-        <f>[1]Inventory!G10</f>
+        <f ca="1">[1]Inventory!G10</f>
         <v>13.3</v>
       </c>
       <c r="H10" t="str">
@@ -1942,33 +1942,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
-        <f>[1]Inventory!A11</f>
+        <f ca="1">[1]Inventory!A11</f>
         <v>CB8NQQ2</v>
       </c>
       <c r="B11" t="str">
-        <f>[1]Inventory!B11</f>
+        <f ca="1">[1]Inventory!B11</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C11" t="str">
-        <f>[1]Inventory!C11</f>
+        <f ca="1">[1]Inventory!C11</f>
         <v>Latitude 5490</v>
       </c>
       <c r="D11" t="str">
-        <f>[1]Inventory!D11</f>
+        <f ca="1">[1]Inventory!D11</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E11">
-        <f>[1]Inventory!E11</f>
+        <f ca="1">[1]Inventory!E11</f>
         <v>8192</v>
       </c>
       <c r="F11" t="str">
-        <f>[1]Inventory!F11</f>
+        <f ca="1">[1]Inventory!F11</f>
         <v>SK hynix SC311 SATA 256GB</v>
       </c>
       <c r="G11">
-        <f>[1]Inventory!G11</f>
+        <f ca="1">[1]Inventory!G11</f>
         <v>13.3</v>
       </c>
       <c r="H11" t="str">
@@ -1976,33 +1976,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
-        <f>[1]Inventory!A12</f>
+        <f ca="1">[1]Inventory!A12</f>
         <v>7KW9QQ2</v>
       </c>
       <c r="B12" t="str">
-        <f>[1]Inventory!B12</f>
+        <f ca="1">[1]Inventory!B12</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C12" t="str">
-        <f>[1]Inventory!C12</f>
+        <f ca="1">[1]Inventory!C12</f>
         <v>Latitude 5490</v>
       </c>
       <c r="D12" t="str">
-        <f>[1]Inventory!D12</f>
+        <f ca="1">[1]Inventory!D12</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E12">
-        <f>[1]Inventory!E12</f>
+        <f ca="1">[1]Inventory!E12</f>
         <v>8192</v>
       </c>
       <c r="F12" t="str">
-        <f>[1]Inventory!F12</f>
+        <f ca="1">[1]Inventory!F12</f>
         <v>TOSHIBA KSG60ZMV256G M.2 2280 256GB</v>
       </c>
       <c r="G12">
-        <f>[1]Inventory!G12</f>
+        <f ca="1">[1]Inventory!G12</f>
         <v>13.3</v>
       </c>
       <c r="H12" t="str">
@@ -2010,33 +2010,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
-        <f>[1]Inventory!A13</f>
+        <f ca="1">[1]Inventory!A13</f>
         <v>38MTNN2</v>
       </c>
       <c r="B13" t="str">
-        <f>[1]Inventory!B13</f>
+        <f ca="1">[1]Inventory!B13</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C13" t="str">
-        <f>[1]Inventory!C13</f>
+        <f ca="1">[1]Inventory!C13</f>
         <v>Latitude 5580</v>
       </c>
       <c r="D13" t="str">
-        <f>[1]Inventory!D13</f>
+        <f ca="1">[1]Inventory!D13</f>
         <v>Intel(R) Core(TM) i5-7300U CPU @ 2.60GHz</v>
       </c>
       <c r="E13">
-        <f>[1]Inventory!E13</f>
+        <f ca="1">[1]Inventory!E13</f>
         <v>16384</v>
       </c>
       <c r="F13" t="str">
-        <f>[1]Inventory!F13</f>
+        <f ca="1">[1]Inventory!F13</f>
         <v>SK hynix SC401 SATA 256GB</v>
       </c>
       <c r="G13">
-        <f>[1]Inventory!G13</f>
+        <f ca="1">[1]Inventory!G13</f>
         <v>15.6</v>
       </c>
       <c r="H13" t="str">
@@ -2044,33 +2044,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
-        <f>[1]Inventory!A14</f>
+        <f ca="1">[1]Inventory!A14</f>
         <v>CVJJMQ2</v>
       </c>
       <c r="B14" t="str">
-        <f>[1]Inventory!B14</f>
+        <f ca="1">[1]Inventory!B14</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C14" t="str">
-        <f>[1]Inventory!C14</f>
+        <f ca="1">[1]Inventory!C14</f>
         <v>Latitude 5590</v>
       </c>
       <c r="D14" t="str">
-        <f>[1]Inventory!D14</f>
+        <f ca="1">[1]Inventory!D14</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E14">
-        <f>[1]Inventory!E14</f>
+        <f ca="1">[1]Inventory!E14</f>
         <v>8192</v>
       </c>
       <c r="F14" t="str">
-        <f>[1]Inventory!F14</f>
+        <f ca="1">[1]Inventory!F14</f>
         <v>WDC WD5000LPLX-75ZNTT0</v>
       </c>
       <c r="G14">
-        <f>[1]Inventory!G14</f>
+        <f ca="1">[1]Inventory!G14</f>
         <v>15.6</v>
       </c>
       <c r="H14" t="str">
@@ -2078,33 +2078,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
-        <f>[1]Inventory!A15</f>
+        <f ca="1">[1]Inventory!A15</f>
         <v>6L6RMQ2</v>
       </c>
       <c r="B15" t="str">
-        <f>[1]Inventory!B15</f>
+        <f ca="1">[1]Inventory!B15</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C15" t="str">
-        <f>[1]Inventory!C15</f>
+        <f ca="1">[1]Inventory!C15</f>
         <v>Latitude 5490</v>
       </c>
       <c r="D15" t="str">
-        <f>[1]Inventory!D15</f>
+        <f ca="1">[1]Inventory!D15</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E15">
-        <f>[1]Inventory!E15</f>
+        <f ca="1">[1]Inventory!E15</f>
         <v>8192</v>
       </c>
       <c r="F15" t="str">
-        <f>[1]Inventory!F15</f>
+        <f ca="1">[1]Inventory!F15</f>
         <v>Micron 1100 SATA 256GB</v>
       </c>
       <c r="G15">
-        <f>[1]Inventory!G15</f>
+        <f ca="1">[1]Inventory!G15</f>
         <v>13.3</v>
       </c>
       <c r="H15" t="str">
@@ -2112,33 +2112,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
-        <f>[1]Inventory!A16</f>
+        <f ca="1">[1]Inventory!A16</f>
         <v>H0J05S2</v>
       </c>
       <c r="B16" t="str">
-        <f>[1]Inventory!B16</f>
+        <f ca="1">[1]Inventory!B16</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C16" t="str">
-        <f>[1]Inventory!C16</f>
+        <f ca="1">[1]Inventory!C16</f>
         <v>Latitude 5490</v>
       </c>
       <c r="D16" t="str">
-        <f>[1]Inventory!D16</f>
+        <f ca="1">[1]Inventory!D16</f>
         <v>Intel(R) Core(TM) i5-8250U CPU @ 1.60GHz</v>
       </c>
       <c r="E16">
-        <f>[1]Inventory!E16</f>
+        <f ca="1">[1]Inventory!E16</f>
         <v>8192</v>
       </c>
       <c r="F16" t="str">
-        <f>[1]Inventory!F16</f>
+        <f ca="1">[1]Inventory!F16</f>
         <v>No drive found</v>
       </c>
       <c r="G16">
-        <f>[1]Inventory!G16</f>
+        <f ca="1">[1]Inventory!G16</f>
         <v>12.5</v>
       </c>
       <c r="H16" t="str">
@@ -2146,33 +2146,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
-        <f>[1]Inventory!A17</f>
+        <f ca="1">[1]Inventory!A17</f>
         <v>JR64Q32</v>
       </c>
       <c r="B17" t="str">
-        <f>[1]Inventory!B17</f>
+        <f ca="1">[1]Inventory!B17</f>
         <v>Dell Inc.</v>
       </c>
       <c r="C17" t="str">
-        <f>[1]Inventory!C17</f>
+        <f ca="1">[1]Inventory!C17</f>
         <v>Latitude E7250</v>
       </c>
       <c r="D17" t="str">
-        <f>[1]Inventory!D17</f>
+        <f ca="1">[1]Inventory!D17</f>
         <v>No CPU found</v>
       </c>
       <c r="E17">
-        <f>[1]Inventory!E17</f>
+        <f ca="1">[1]Inventory!E17</f>
         <v>8192</v>
       </c>
       <c r="F17" t="str">
-        <f>[1]Inventory!F17</f>
+        <f ca="1">[1]Inventory!F17</f>
         <v>No drive found</v>
       </c>
       <c r="G17">
-        <f>[1]Inventory!G17</f>
+        <f ca="1">[1]Inventory!G17</f>
         <v>12.5</v>
       </c>
       <c r="H17" t="str">
@@ -2180,33 +2180,33 @@
         <v>GOOD</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
-        <f>[1]Inventory!A18</f>
+        <f ca="1">[1]Inventory!A18</f>
         <v>0</v>
       </c>
       <c r="B18">
-        <f>[1]Inventory!B18</f>
+        <f ca="1">[1]Inventory!B18</f>
         <v>0</v>
       </c>
       <c r="C18">
-        <f>[1]Inventory!C18</f>
+        <f ca="1">[1]Inventory!C18</f>
         <v>0</v>
       </c>
       <c r="D18">
-        <f>[1]Inventory!D18</f>
+        <f ca="1">[1]Inventory!D18</f>
         <v>0</v>
       </c>
       <c r="E18">
-        <f>[1]Inventory!E18</f>
+        <f ca="1">[1]Inventory!E18</f>
         <v>0</v>
       </c>
       <c r="F18">
-        <f>[1]Inventory!F18</f>
+        <f ca="1">[1]Inventory!F18</f>
         <v>0</v>
       </c>
       <c r="G18">
-        <f>[1]Inventory!G18</f>
+        <f ca="1">[1]Inventory!G18</f>
         <v>0</v>
       </c>
       <c r="H18" t="str">
@@ -2214,33 +2214,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
-        <f>[1]Inventory!A19</f>
+        <f ca="1">[1]Inventory!A19</f>
         <v>0</v>
       </c>
       <c r="B19">
-        <f>[1]Inventory!B19</f>
+        <f ca="1">[1]Inventory!B19</f>
         <v>0</v>
       </c>
       <c r="C19">
-        <f>[1]Inventory!C19</f>
+        <f ca="1">[1]Inventory!C19</f>
         <v>0</v>
       </c>
       <c r="D19">
-        <f>[1]Inventory!D19</f>
+        <f ca="1">[1]Inventory!D19</f>
         <v>0</v>
       </c>
       <c r="E19">
-        <f>[1]Inventory!E19</f>
+        <f ca="1">[1]Inventory!E19</f>
         <v>0</v>
       </c>
       <c r="F19">
-        <f>[1]Inventory!F19</f>
+        <f ca="1">[1]Inventory!F19</f>
         <v>0</v>
       </c>
       <c r="G19">
-        <f>[1]Inventory!G19</f>
+        <f ca="1">[1]Inventory!G19</f>
         <v>0</v>
       </c>
       <c r="H19" t="str">
@@ -2248,33 +2248,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
-        <f>[1]Inventory!A20</f>
+        <f ca="1">[1]Inventory!A20</f>
         <v>0</v>
       </c>
       <c r="B20">
-        <f>[1]Inventory!B20</f>
+        <f ca="1">[1]Inventory!B20</f>
         <v>0</v>
       </c>
       <c r="C20">
-        <f>[1]Inventory!C20</f>
+        <f ca="1">[1]Inventory!C20</f>
         <v>0</v>
       </c>
       <c r="D20">
-        <f>[1]Inventory!D20</f>
+        <f ca="1">[1]Inventory!D20</f>
         <v>0</v>
       </c>
       <c r="E20">
-        <f>[1]Inventory!E20</f>
+        <f ca="1">[1]Inventory!E20</f>
         <v>0</v>
       </c>
       <c r="F20">
-        <f>[1]Inventory!F20</f>
+        <f ca="1">[1]Inventory!F20</f>
         <v>0</v>
       </c>
       <c r="G20">
-        <f>[1]Inventory!G20</f>
+        <f ca="1">[1]Inventory!G20</f>
         <v>0</v>
       </c>
       <c r="H20" t="str">
@@ -2282,33 +2282,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
-        <f>[1]Inventory!A21</f>
+        <f ca="1">[1]Inventory!A21</f>
         <v>0</v>
       </c>
       <c r="B21">
-        <f>[1]Inventory!B21</f>
+        <f ca="1">[1]Inventory!B21</f>
         <v>0</v>
       </c>
       <c r="C21">
-        <f>[1]Inventory!C21</f>
+        <f ca="1">[1]Inventory!C21</f>
         <v>0</v>
       </c>
       <c r="D21">
-        <f>[1]Inventory!D21</f>
+        <f ca="1">[1]Inventory!D21</f>
         <v>0</v>
       </c>
       <c r="E21">
-        <f>[1]Inventory!E21</f>
+        <f ca="1">[1]Inventory!E21</f>
         <v>0</v>
       </c>
       <c r="F21">
-        <f>[1]Inventory!F21</f>
+        <f ca="1">[1]Inventory!F21</f>
         <v>0</v>
       </c>
       <c r="G21">
-        <f>[1]Inventory!G21</f>
+        <f ca="1">[1]Inventory!G21</f>
         <v>0</v>
       </c>
       <c r="H21" t="str">
@@ -2316,33 +2316,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
-        <f>[1]Inventory!A22</f>
+        <f ca="1">[1]Inventory!A22</f>
         <v>0</v>
       </c>
       <c r="B22">
-        <f>[1]Inventory!B22</f>
+        <f ca="1">[1]Inventory!B22</f>
         <v>0</v>
       </c>
       <c r="C22">
-        <f>[1]Inventory!C22</f>
+        <f ca="1">[1]Inventory!C22</f>
         <v>0</v>
       </c>
       <c r="D22">
-        <f>[1]Inventory!D22</f>
+        <f ca="1">[1]Inventory!D22</f>
         <v>0</v>
       </c>
       <c r="E22">
-        <f>[1]Inventory!E22</f>
+        <f ca="1">[1]Inventory!E22</f>
         <v>0</v>
       </c>
       <c r="F22">
-        <f>[1]Inventory!F22</f>
+        <f ca="1">[1]Inventory!F22</f>
         <v>0</v>
       </c>
       <c r="G22">
-        <f>[1]Inventory!G22</f>
+        <f ca="1">[1]Inventory!G22</f>
         <v>0</v>
       </c>
       <c r="H22" t="str">
@@ -2350,33 +2350,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
-        <f>[1]Inventory!A23</f>
+        <f ca="1">[1]Inventory!A23</f>
         <v>0</v>
       </c>
       <c r="B23">
-        <f>[1]Inventory!B23</f>
+        <f ca="1">[1]Inventory!B23</f>
         <v>0</v>
       </c>
       <c r="C23">
-        <f>[1]Inventory!C23</f>
+        <f ca="1">[1]Inventory!C23</f>
         <v>0</v>
       </c>
       <c r="D23">
-        <f>[1]Inventory!D23</f>
+        <f ca="1">[1]Inventory!D23</f>
         <v>0</v>
       </c>
       <c r="E23">
-        <f>[1]Inventory!E23</f>
+        <f ca="1">[1]Inventory!E23</f>
         <v>0</v>
       </c>
       <c r="F23">
-        <f>[1]Inventory!F23</f>
+        <f ca="1">[1]Inventory!F23</f>
         <v>0</v>
       </c>
       <c r="G23">
-        <f>[1]Inventory!G23</f>
+        <f ca="1">[1]Inventory!G23</f>
         <v>0</v>
       </c>
       <c r="H23" t="str">
@@ -2384,33 +2384,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
-        <f>[1]Inventory!A24</f>
+        <f ca="1">[1]Inventory!A24</f>
         <v>0</v>
       </c>
       <c r="B24">
-        <f>[1]Inventory!B24</f>
+        <f ca="1">[1]Inventory!B24</f>
         <v>0</v>
       </c>
       <c r="C24">
-        <f>[1]Inventory!C24</f>
+        <f ca="1">[1]Inventory!C24</f>
         <v>0</v>
       </c>
       <c r="D24">
-        <f>[1]Inventory!D24</f>
+        <f ca="1">[1]Inventory!D24</f>
         <v>0</v>
       </c>
       <c r="E24">
-        <f>[1]Inventory!E24</f>
+        <f ca="1">[1]Inventory!E24</f>
         <v>0</v>
       </c>
       <c r="F24">
-        <f>[1]Inventory!F24</f>
+        <f ca="1">[1]Inventory!F24</f>
         <v>0</v>
       </c>
       <c r="G24">
-        <f>[1]Inventory!G24</f>
+        <f ca="1">[1]Inventory!G24</f>
         <v>0</v>
       </c>
       <c r="H24" t="str">
@@ -2418,33 +2418,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
-        <f>[1]Inventory!A25</f>
+        <f ca="1">[1]Inventory!A25</f>
         <v>0</v>
       </c>
       <c r="B25">
-        <f>[1]Inventory!B25</f>
+        <f ca="1">[1]Inventory!B25</f>
         <v>0</v>
       </c>
       <c r="C25">
-        <f>[1]Inventory!C25</f>
+        <f ca="1">[1]Inventory!C25</f>
         <v>0</v>
       </c>
       <c r="D25">
-        <f>[1]Inventory!D25</f>
+        <f ca="1">[1]Inventory!D25</f>
         <v>0</v>
       </c>
       <c r="E25">
-        <f>[1]Inventory!E25</f>
+        <f ca="1">[1]Inventory!E25</f>
         <v>0</v>
       </c>
       <c r="F25">
-        <f>[1]Inventory!F25</f>
+        <f ca="1">[1]Inventory!F25</f>
         <v>0</v>
       </c>
       <c r="G25">
-        <f>[1]Inventory!G25</f>
+        <f ca="1">[1]Inventory!G25</f>
         <v>0</v>
       </c>
       <c r="H25" t="str">
@@ -2452,33 +2452,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
-        <f>[1]Inventory!A26</f>
+        <f ca="1">[1]Inventory!A26</f>
         <v>0</v>
       </c>
       <c r="B26">
-        <f>[1]Inventory!B26</f>
+        <f ca="1">[1]Inventory!B26</f>
         <v>0</v>
       </c>
       <c r="C26">
-        <f>[1]Inventory!C26</f>
+        <f ca="1">[1]Inventory!C26</f>
         <v>0</v>
       </c>
       <c r="D26">
-        <f>[1]Inventory!D26</f>
+        <f ca="1">[1]Inventory!D26</f>
         <v>0</v>
       </c>
       <c r="E26">
-        <f>[1]Inventory!E26</f>
+        <f ca="1">[1]Inventory!E26</f>
         <v>0</v>
       </c>
       <c r="F26">
-        <f>[1]Inventory!F26</f>
+        <f ca="1">[1]Inventory!F26</f>
         <v>0</v>
       </c>
       <c r="G26">
-        <f>[1]Inventory!G26</f>
+        <f ca="1">[1]Inventory!G26</f>
         <v>0</v>
       </c>
       <c r="H26" t="str">
@@ -2486,33 +2486,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
-        <f>[1]Inventory!A27</f>
+        <f ca="1">[1]Inventory!A27</f>
         <v>0</v>
       </c>
       <c r="B27">
-        <f>[1]Inventory!B27</f>
+        <f ca="1">[1]Inventory!B27</f>
         <v>0</v>
       </c>
       <c r="C27">
-        <f>[1]Inventory!C27</f>
+        <f ca="1">[1]Inventory!C27</f>
         <v>0</v>
       </c>
       <c r="D27">
-        <f>[1]Inventory!D27</f>
+        <f ca="1">[1]Inventory!D27</f>
         <v>0</v>
       </c>
       <c r="E27">
-        <f>[1]Inventory!E27</f>
+        <f ca="1">[1]Inventory!E27</f>
         <v>0</v>
       </c>
       <c r="F27">
-        <f>[1]Inventory!F27</f>
+        <f ca="1">[1]Inventory!F27</f>
         <v>0</v>
       </c>
       <c r="G27">
-        <f>[1]Inventory!G27</f>
+        <f ca="1">[1]Inventory!G27</f>
         <v>0</v>
       </c>
       <c r="H27" t="str">
@@ -2520,33 +2520,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
-        <f>[1]Inventory!A28</f>
+        <f ca="1">[1]Inventory!A28</f>
         <v>0</v>
       </c>
       <c r="B28">
-        <f>[1]Inventory!B28</f>
+        <f ca="1">[1]Inventory!B28</f>
         <v>0</v>
       </c>
       <c r="C28">
-        <f>[1]Inventory!C28</f>
+        <f ca="1">[1]Inventory!C28</f>
         <v>0</v>
       </c>
       <c r="D28">
-        <f>[1]Inventory!D28</f>
+        <f ca="1">[1]Inventory!D28</f>
         <v>0</v>
       </c>
       <c r="E28">
-        <f>[1]Inventory!E28</f>
+        <f ca="1">[1]Inventory!E28</f>
         <v>0</v>
       </c>
       <c r="F28">
-        <f>[1]Inventory!F28</f>
+        <f ca="1">[1]Inventory!F28</f>
         <v>0</v>
       </c>
       <c r="G28">
-        <f>[1]Inventory!G28</f>
+        <f ca="1">[1]Inventory!G28</f>
         <v>0</v>
       </c>
       <c r="H28" t="str">
@@ -2554,33 +2554,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
-        <f>[1]Inventory!A29</f>
+        <f ca="1">[1]Inventory!A29</f>
         <v>0</v>
       </c>
       <c r="B29">
-        <f>[1]Inventory!B29</f>
+        <f ca="1">[1]Inventory!B29</f>
         <v>0</v>
       </c>
       <c r="C29">
-        <f>[1]Inventory!C29</f>
+        <f ca="1">[1]Inventory!C29</f>
         <v>0</v>
       </c>
       <c r="D29">
-        <f>[1]Inventory!D29</f>
+        <f ca="1">[1]Inventory!D29</f>
         <v>0</v>
       </c>
       <c r="E29">
-        <f>[1]Inventory!E29</f>
+        <f ca="1">[1]Inventory!E29</f>
         <v>0</v>
       </c>
       <c r="F29">
-        <f>[1]Inventory!F29</f>
+        <f ca="1">[1]Inventory!F29</f>
         <v>0</v>
       </c>
       <c r="G29">
-        <f>[1]Inventory!G29</f>
+        <f ca="1">[1]Inventory!G29</f>
         <v>0</v>
       </c>
       <c r="H29" t="str">
@@ -2588,33 +2588,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30">
-        <f>[1]Inventory!A30</f>
+        <f ca="1">[1]Inventory!A30</f>
         <v>0</v>
       </c>
       <c r="B30">
-        <f>[1]Inventory!B30</f>
+        <f ca="1">[1]Inventory!B30</f>
         <v>0</v>
       </c>
       <c r="C30">
-        <f>[1]Inventory!C30</f>
+        <f ca="1">[1]Inventory!C30</f>
         <v>0</v>
       </c>
       <c r="D30">
-        <f>[1]Inventory!D30</f>
+        <f ca="1">[1]Inventory!D30</f>
         <v>0</v>
       </c>
       <c r="E30">
-        <f>[1]Inventory!E30</f>
+        <f ca="1">[1]Inventory!E30</f>
         <v>0</v>
       </c>
       <c r="F30">
-        <f>[1]Inventory!F30</f>
+        <f ca="1">[1]Inventory!F30</f>
         <v>0</v>
       </c>
       <c r="G30">
-        <f>[1]Inventory!G30</f>
+        <f ca="1">[1]Inventory!G30</f>
         <v>0</v>
       </c>
       <c r="H30" t="str">
@@ -2622,33 +2622,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
-        <f>[1]Inventory!A31</f>
+        <f ca="1">[1]Inventory!A31</f>
         <v>0</v>
       </c>
       <c r="B31">
-        <f>[1]Inventory!B31</f>
+        <f ca="1">[1]Inventory!B31</f>
         <v>0</v>
       </c>
       <c r="C31">
-        <f>[1]Inventory!C31</f>
+        <f ca="1">[1]Inventory!C31</f>
         <v>0</v>
       </c>
       <c r="D31">
-        <f>[1]Inventory!D31</f>
+        <f ca="1">[1]Inventory!D31</f>
         <v>0</v>
       </c>
       <c r="E31">
-        <f>[1]Inventory!E31</f>
+        <f ca="1">[1]Inventory!E31</f>
         <v>0</v>
       </c>
       <c r="F31">
-        <f>[1]Inventory!F31</f>
+        <f ca="1">[1]Inventory!F31</f>
         <v>0</v>
       </c>
       <c r="G31">
-        <f>[1]Inventory!G31</f>
+        <f ca="1">[1]Inventory!G31</f>
         <v>0</v>
       </c>
       <c r="H31" t="str">
@@ -2656,33 +2656,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32">
-        <f>[1]Inventory!A32</f>
+        <f ca="1">[1]Inventory!A32</f>
         <v>0</v>
       </c>
       <c r="B32">
-        <f>[1]Inventory!B32</f>
+        <f ca="1">[1]Inventory!B32</f>
         <v>0</v>
       </c>
       <c r="C32">
-        <f>[1]Inventory!C32</f>
+        <f ca="1">[1]Inventory!C32</f>
         <v>0</v>
       </c>
       <c r="D32">
-        <f>[1]Inventory!D32</f>
+        <f ca="1">[1]Inventory!D32</f>
         <v>0</v>
       </c>
       <c r="E32">
-        <f>[1]Inventory!E32</f>
+        <f ca="1">[1]Inventory!E32</f>
         <v>0</v>
       </c>
       <c r="F32">
-        <f>[1]Inventory!F32</f>
+        <f ca="1">[1]Inventory!F32</f>
         <v>0</v>
       </c>
       <c r="G32">
-        <f>[1]Inventory!G32</f>
+        <f ca="1">[1]Inventory!G32</f>
         <v>0</v>
       </c>
       <c r="H32" t="str">
@@ -2690,33 +2690,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33">
-        <f>[1]Inventory!A33</f>
+        <f ca="1">[1]Inventory!A33</f>
         <v>0</v>
       </c>
       <c r="B33">
-        <f>[1]Inventory!B33</f>
+        <f ca="1">[1]Inventory!B33</f>
         <v>0</v>
       </c>
       <c r="C33">
-        <f>[1]Inventory!C33</f>
+        <f ca="1">[1]Inventory!C33</f>
         <v>0</v>
       </c>
       <c r="D33">
-        <f>[1]Inventory!D33</f>
+        <f ca="1">[1]Inventory!D33</f>
         <v>0</v>
       </c>
       <c r="E33">
-        <f>[1]Inventory!E33</f>
+        <f ca="1">[1]Inventory!E33</f>
         <v>0</v>
       </c>
       <c r="F33">
-        <f>[1]Inventory!F33</f>
+        <f ca="1">[1]Inventory!F33</f>
         <v>0</v>
       </c>
       <c r="G33">
-        <f>[1]Inventory!G33</f>
+        <f ca="1">[1]Inventory!G33</f>
         <v>0</v>
       </c>
       <c r="H33" t="str">
@@ -2724,33 +2724,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34">
-        <f>[1]Inventory!A34</f>
+        <f ca="1">[1]Inventory!A34</f>
         <v>0</v>
       </c>
       <c r="B34">
-        <f>[1]Inventory!B34</f>
+        <f ca="1">[1]Inventory!B34</f>
         <v>0</v>
       </c>
       <c r="C34">
-        <f>[1]Inventory!C34</f>
+        <f ca="1">[1]Inventory!C34</f>
         <v>0</v>
       </c>
       <c r="D34">
-        <f>[1]Inventory!D34</f>
+        <f ca="1">[1]Inventory!D34</f>
         <v>0</v>
       </c>
       <c r="E34">
-        <f>[1]Inventory!E34</f>
+        <f ca="1">[1]Inventory!E34</f>
         <v>0</v>
       </c>
       <c r="F34">
-        <f>[1]Inventory!F34</f>
+        <f ca="1">[1]Inventory!F34</f>
         <v>0</v>
       </c>
       <c r="G34">
-        <f>[1]Inventory!G34</f>
+        <f ca="1">[1]Inventory!G34</f>
         <v>0</v>
       </c>
       <c r="H34" t="str">
@@ -2758,33 +2758,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35">
-        <f>[1]Inventory!A35</f>
+        <f ca="1">[1]Inventory!A35</f>
         <v>0</v>
       </c>
       <c r="B35">
-        <f>[1]Inventory!B35</f>
+        <f ca="1">[1]Inventory!B35</f>
         <v>0</v>
       </c>
       <c r="C35">
-        <f>[1]Inventory!C35</f>
+        <f ca="1">[1]Inventory!C35</f>
         <v>0</v>
       </c>
       <c r="D35">
-        <f>[1]Inventory!D35</f>
+        <f ca="1">[1]Inventory!D35</f>
         <v>0</v>
       </c>
       <c r="E35">
-        <f>[1]Inventory!E35</f>
+        <f ca="1">[1]Inventory!E35</f>
         <v>0</v>
       </c>
       <c r="F35">
-        <f>[1]Inventory!F35</f>
+        <f ca="1">[1]Inventory!F35</f>
         <v>0</v>
       </c>
       <c r="G35">
-        <f>[1]Inventory!G35</f>
+        <f ca="1">[1]Inventory!G35</f>
         <v>0</v>
       </c>
       <c r="H35" t="str">
@@ -2792,33 +2792,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36">
-        <f>[1]Inventory!A36</f>
+        <f ca="1">[1]Inventory!A36</f>
         <v>0</v>
       </c>
       <c r="B36">
-        <f>[1]Inventory!B36</f>
+        <f ca="1">[1]Inventory!B36</f>
         <v>0</v>
       </c>
       <c r="C36">
-        <f>[1]Inventory!C36</f>
+        <f ca="1">[1]Inventory!C36</f>
         <v>0</v>
       </c>
       <c r="D36">
-        <f>[1]Inventory!D36</f>
+        <f ca="1">[1]Inventory!D36</f>
         <v>0</v>
       </c>
       <c r="E36">
-        <f>[1]Inventory!E36</f>
+        <f ca="1">[1]Inventory!E36</f>
         <v>0</v>
       </c>
       <c r="F36">
-        <f>[1]Inventory!F36</f>
+        <f ca="1">[1]Inventory!F36</f>
         <v>0</v>
       </c>
       <c r="G36">
-        <f>[1]Inventory!G36</f>
+        <f ca="1">[1]Inventory!G36</f>
         <v>0</v>
       </c>
       <c r="H36" t="str">
@@ -2826,33 +2826,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
-        <f>[1]Inventory!A37</f>
+        <f ca="1">[1]Inventory!A37</f>
         <v>0</v>
       </c>
       <c r="B37">
-        <f>[1]Inventory!B37</f>
+        <f ca="1">[1]Inventory!B37</f>
         <v>0</v>
       </c>
       <c r="C37">
-        <f>[1]Inventory!C37</f>
+        <f ca="1">[1]Inventory!C37</f>
         <v>0</v>
       </c>
       <c r="D37">
-        <f>[1]Inventory!D37</f>
+        <f ca="1">[1]Inventory!D37</f>
         <v>0</v>
       </c>
       <c r="E37">
-        <f>[1]Inventory!E37</f>
+        <f ca="1">[1]Inventory!E37</f>
         <v>0</v>
       </c>
       <c r="F37">
-        <f>[1]Inventory!F37</f>
+        <f ca="1">[1]Inventory!F37</f>
         <v>0</v>
       </c>
       <c r="G37">
-        <f>[1]Inventory!G37</f>
+        <f ca="1">[1]Inventory!G37</f>
         <v>0</v>
       </c>
       <c r="H37" t="str">
@@ -2860,33 +2860,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38">
-        <f>[1]Inventory!A38</f>
+        <f ca="1">[1]Inventory!A38</f>
         <v>0</v>
       </c>
       <c r="B38">
-        <f>[1]Inventory!B38</f>
+        <f ca="1">[1]Inventory!B38</f>
         <v>0</v>
       </c>
       <c r="C38">
-        <f>[1]Inventory!C38</f>
+        <f ca="1">[1]Inventory!C38</f>
         <v>0</v>
       </c>
       <c r="D38">
-        <f>[1]Inventory!D38</f>
+        <f ca="1">[1]Inventory!D38</f>
         <v>0</v>
       </c>
       <c r="E38">
-        <f>[1]Inventory!E38</f>
+        <f ca="1">[1]Inventory!E38</f>
         <v>0</v>
       </c>
       <c r="F38">
-        <f>[1]Inventory!F38</f>
+        <f ca="1">[1]Inventory!F38</f>
         <v>0</v>
       </c>
       <c r="G38">
-        <f>[1]Inventory!G38</f>
+        <f ca="1">[1]Inventory!G38</f>
         <v>0</v>
       </c>
       <c r="H38" t="str">
@@ -2894,33 +2894,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39">
-        <f>[1]Inventory!A39</f>
+        <f ca="1">[1]Inventory!A39</f>
         <v>0</v>
       </c>
       <c r="B39">
-        <f>[1]Inventory!B39</f>
+        <f ca="1">[1]Inventory!B39</f>
         <v>0</v>
       </c>
       <c r="C39">
-        <f>[1]Inventory!C39</f>
+        <f ca="1">[1]Inventory!C39</f>
         <v>0</v>
       </c>
       <c r="D39">
-        <f>[1]Inventory!D39</f>
+        <f ca="1">[1]Inventory!D39</f>
         <v>0</v>
       </c>
       <c r="E39">
-        <f>[1]Inventory!E39</f>
+        <f ca="1">[1]Inventory!E39</f>
         <v>0</v>
       </c>
       <c r="F39">
-        <f>[1]Inventory!F39</f>
+        <f ca="1">[1]Inventory!F39</f>
         <v>0</v>
       </c>
       <c r="G39">
-        <f>[1]Inventory!G39</f>
+        <f ca="1">[1]Inventory!G39</f>
         <v>0</v>
       </c>
       <c r="H39" t="str">
@@ -2928,33 +2928,33 @@
         <v>BAD</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40">
-        <f>[1]Inventory!A40</f>
+        <f ca="1">[1]Inventory!A40</f>
         <v>0</v>
       </c>
       <c r="B40">
-        <f>[1]Inventory!B40</f>
+        <f ca="1">[1]Inventory!B40</f>
         <v>0</v>
       </c>
       <c r="C40">
-        <f>[1]Inventory!C40</f>
+        <f ca="1">[1]Inventory!C40</f>
         <v>0</v>
       </c>
       <c r="D40">
-        <f>[1]Inventory!D40</f>
+        <f ca="1">[1]Inventory!D40</f>
         <v>0</v>
       </c>
       <c r="E40">
-        <f>[1]Inventory!E40</f>
+        <f ca="1">[1]Inventory!E40</f>
         <v>0</v>
       </c>
       <c r="F40">
-        <f>[1]Inventory!F40</f>
+        <f ca="1">[1]Inventory!F40</f>
         <v>0</v>
       </c>
       <c r="G40">
-        <f>[1]Inventory!G40</f>
+        <f ca="1">[1]Inventory!G40</f>
         <v>0</v>
       </c>
       <c r="H40" t="str">
@@ -2983,15 +2983,15 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="67.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="67.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
-        <f>Inventory!A1</f>
+        <f ca="1">Inventory!A1</f>
         <v>Serial</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -3019,9 +3019,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
-        <f>Inventory!A2</f>
+        <f ca="1">Inventory!A2</f>
         <v>9442Q32</v>
       </c>
       <c r="B2" t="s">
@@ -3046,9 +3046,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
-        <f>Inventory!A3</f>
+        <f ca="1">Inventory!A3</f>
         <v>J703QV2</v>
       </c>
       <c r="B3" t="s">
@@ -3076,9 +3076,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
-        <f>Inventory!A4</f>
+        <f ca="1">Inventory!A4</f>
         <v>FJ9QLQ2</v>
       </c>
       <c r="B4" t="s">
@@ -3103,13 +3103,13 @@
         <v>39</v>
       </c>
       <c r="I4" t="str">
-        <f>[1]Inventory!H4</f>
+        <f ca="1">[1]Inventory!H4</f>
         <v>No battery; bad trackpad</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
-        <f>Inventory!A5</f>
+        <f ca="1">Inventory!A5</f>
         <v>H4RFJR2</v>
       </c>
       <c r="B5" t="s">
@@ -3134,13 +3134,13 @@
         <v>40</v>
       </c>
       <c r="I5" t="str">
-        <f>[1]Inventory!H5</f>
+        <f ca="1">[1]Inventory!H5</f>
         <v>Bad battery; random shutdowns; no esc key</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
-        <f>Inventory!A6</f>
+        <f ca="1">Inventory!A6</f>
         <v>BBMJLQ2</v>
       </c>
       <c r="B6" t="s">
@@ -3165,13 +3165,13 @@
         <v>39</v>
       </c>
       <c r="I6" t="str">
-        <f>[1]Inventory!H6</f>
+        <f ca="1">[1]Inventory!H6</f>
         <v>No battery; no hdd</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
-        <f>Inventory!A7</f>
+        <f ca="1">Inventory!A7</f>
         <v>HRQBQV2</v>
       </c>
       <c r="B7" t="s">
@@ -3196,13 +3196,13 @@
         <v>39</v>
       </c>
       <c r="I7" t="str">
-        <f>[1]Inventory!H7</f>
+        <f ca="1">[1]Inventory!H7</f>
         <v>No battery; USB-C cosmetic damage</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
-        <f>Inventory!A8</f>
+        <f ca="1">Inventory!A8</f>
         <v>C484M12</v>
       </c>
       <c r="B8" t="s">
@@ -3227,13 +3227,13 @@
         <v>39</v>
       </c>
       <c r="I8" t="str">
-        <f>[1]Inventory!H8</f>
+        <f ca="1">[1]Inventory!H8</f>
         <v>Needs cleaning and check</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
-        <f>Inventory!A9</f>
+        <f ca="1">Inventory!A9</f>
         <v>29VM533</v>
       </c>
       <c r="B9" t="s">
@@ -3258,13 +3258,13 @@
         <v>39</v>
       </c>
       <c r="I9" t="str">
-        <f>[1]Inventory!H9</f>
+        <f ca="1">[1]Inventory!H9</f>
         <v>No battery; bad screen</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
-        <f>Inventory!A10</f>
+        <f ca="1">Inventory!A10</f>
         <v>5DRF3M2</v>
       </c>
       <c r="B10" t="s">
@@ -3289,13 +3289,13 @@
         <v>39</v>
       </c>
       <c r="I10" t="str">
-        <f>[1]Inventory!H10</f>
+        <f ca="1">[1]Inventory!H10</f>
         <v>No battery; bad hdd</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
-        <f>Inventory!A11</f>
+        <f ca="1">Inventory!A11</f>
         <v>CB8NQQ2</v>
       </c>
       <c r="B11" t="s">
@@ -3320,13 +3320,13 @@
         <v>39</v>
       </c>
       <c r="I11" t="str">
-        <f>[1]Inventory!H11</f>
+        <f ca="1">[1]Inventory!H11</f>
         <v>No battery; no ram; bad keyboard</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
-        <f>Inventory!A12</f>
+        <f ca="1">Inventory!A12</f>
         <v>7KW9QQ2</v>
       </c>
       <c r="B12" t="s">
@@ -3351,13 +3351,13 @@
         <v>40</v>
       </c>
       <c r="I12" t="str">
-        <f>[1]Inventory!H12</f>
+        <f ca="1">[1]Inventory!H12</f>
         <v>No battery; bad keyboard; front cover bulge; bad drivers</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
-        <f>Inventory!A13</f>
+        <f ca="1">Inventory!A13</f>
         <v>38MTNN2</v>
       </c>
       <c r="B13" t="s">
@@ -3382,13 +3382,13 @@
         <v>39</v>
       </c>
       <c r="I13" t="str">
-        <f>[1]Inventory!H13</f>
+        <f ca="1">[1]Inventory!H13</f>
         <v>No battery; no ram; bad ethernet; ALIAS VMNB0128</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
-        <f>Inventory!A14</f>
+        <f ca="1">Inventory!A14</f>
         <v>CVJJMQ2</v>
       </c>
       <c r="B14" t="s">
@@ -3413,13 +3413,13 @@
         <v>39</v>
       </c>
       <c r="I14" t="str">
-        <f>[1]Inventory!H14</f>
+        <f ca="1">[1]Inventory!H14</f>
         <v>No battery; ALIAS VMNB0131</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
-        <f>Inventory!A15</f>
+        <f ca="1">Inventory!A15</f>
         <v>6L6RMQ2</v>
       </c>
       <c r="B15" t="s">
@@ -3444,13 +3444,13 @@
         <v>39</v>
       </c>
       <c r="I15" t="str">
-        <f>[1]Inventory!H15</f>
+        <f ca="1">[1]Inventory!H15</f>
         <v>No battery; no j key or joystick; no trackpad buttons</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
-        <f>Inventory!A16</f>
+        <f ca="1">Inventory!A16</f>
         <v>H0J05S2</v>
       </c>
       <c r="B16" t="s">
@@ -3475,13 +3475,13 @@
         <v>40</v>
       </c>
       <c r="I16" t="str">
-        <f>[1]Inventory!H16</f>
+        <f ca="1">[1]Inventory!H16</f>
         <v>Don't even bother</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
-        <f>Inventory!A17</f>
+        <f ca="1">Inventory!A17</f>
         <v>JR64Q32</v>
       </c>
       <c r="B17" t="s">
@@ -3506,1047 +3506,1047 @@
         <v>39</v>
       </c>
       <c r="I17" t="str">
-        <f>[1]Inventory!H17</f>
+        <f ca="1">[1]Inventory!H17</f>
         <v>Needs check</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
-        <f>Inventory!A18</f>
+        <f ca="1">Inventory!A18</f>
         <v>0</v>
       </c>
       <c r="I18">
-        <f>[1]Inventory!H18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
-        <f>Inventory!A19</f>
+        <f ca="1">Inventory!A19</f>
         <v>0</v>
       </c>
       <c r="I19">
-        <f>[1]Inventory!H19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
-        <f>Inventory!A20</f>
+        <f ca="1">Inventory!A20</f>
         <v>0</v>
       </c>
       <c r="I20">
-        <f>[1]Inventory!H20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
-        <f>Inventory!A21</f>
+        <f ca="1">Inventory!A21</f>
         <v>0</v>
       </c>
       <c r="I21">
-        <f>[1]Inventory!H21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
-        <f>Inventory!A22</f>
+        <f ca="1">Inventory!A22</f>
         <v>0</v>
       </c>
       <c r="I22">
-        <f>[1]Inventory!H22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
-        <f>Inventory!A23</f>
+        <f ca="1">Inventory!A23</f>
         <v>0</v>
       </c>
       <c r="I23">
-        <f>[1]Inventory!H23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
-        <f>Inventory!A24</f>
+        <f ca="1">Inventory!A24</f>
         <v>0</v>
       </c>
       <c r="I24">
-        <f>[1]Inventory!H24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
-        <f>Inventory!A25</f>
+        <f ca="1">Inventory!A25</f>
         <v>0</v>
       </c>
       <c r="I25">
-        <f>[1]Inventory!H25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
-        <f>Inventory!A26</f>
+        <f ca="1">Inventory!A26</f>
         <v>0</v>
       </c>
       <c r="I26">
-        <f>[1]Inventory!H26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
-        <f>Inventory!A27</f>
+        <f ca="1">Inventory!A27</f>
         <v>0</v>
       </c>
       <c r="I27">
-        <f>[1]Inventory!H27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
-        <f>Inventory!A28</f>
+        <f ca="1">Inventory!A28</f>
         <v>0</v>
       </c>
       <c r="I28">
-        <f>[1]Inventory!H28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
-        <f>Inventory!A29</f>
+        <f ca="1">Inventory!A29</f>
         <v>0</v>
       </c>
       <c r="I29">
-        <f>[1]Inventory!H29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
-        <f>Inventory!A30</f>
+        <f ca="1">Inventory!A30</f>
         <v>0</v>
       </c>
       <c r="I30">
-        <f>[1]Inventory!H30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
-        <f>Inventory!A31</f>
+        <f ca="1">Inventory!A31</f>
         <v>0</v>
       </c>
       <c r="I31">
-        <f>[1]Inventory!H31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
-        <f>Inventory!A32</f>
+        <f ca="1">Inventory!A32</f>
         <v>0</v>
       </c>
       <c r="I32">
-        <f>[1]Inventory!H32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
-        <f>Inventory!A33</f>
+        <f ca="1">Inventory!A33</f>
         <v>0</v>
       </c>
       <c r="I33">
-        <f>[1]Inventory!H33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
-        <f>Inventory!A34</f>
+        <f ca="1">Inventory!A34</f>
         <v>0</v>
       </c>
       <c r="I34">
-        <f>[1]Inventory!H34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
-        <f>Inventory!A35</f>
+        <f ca="1">Inventory!A35</f>
         <v>0</v>
       </c>
       <c r="I35">
-        <f>[1]Inventory!H35</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
-        <f>Inventory!A36</f>
+        <f ca="1">Inventory!A36</f>
         <v>0</v>
       </c>
       <c r="I36">
-        <f>[1]Inventory!H36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
-        <f>Inventory!A37</f>
+        <f ca="1">Inventory!A37</f>
         <v>0</v>
       </c>
       <c r="I37">
-        <f>[1]Inventory!H37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
-        <f>Inventory!A38</f>
+        <f ca="1">Inventory!A38</f>
         <v>0</v>
       </c>
       <c r="I38">
-        <f>[1]Inventory!H38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
-        <f>Inventory!A39</f>
+        <f ca="1">Inventory!A39</f>
         <v>0</v>
       </c>
       <c r="I39">
-        <f>[1]Inventory!H39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
-        <f>Inventory!A40</f>
+        <f ca="1">Inventory!A40</f>
         <v>0</v>
       </c>
       <c r="I40">
-        <f>[1]Inventory!H40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <f>Inventory!A41</f>
         <v>0</v>
       </c>
       <c r="I41">
-        <f>[1]Inventory!H41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <f>Inventory!A42</f>
         <v>0</v>
       </c>
       <c r="I42">
-        <f>[1]Inventory!H42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <f>Inventory!A43</f>
         <v>0</v>
       </c>
       <c r="I43">
-        <f>[1]Inventory!H43</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <f>Inventory!A44</f>
         <v>0</v>
       </c>
       <c r="I44">
-        <f>[1]Inventory!H44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <f>Inventory!A45</f>
         <v>0</v>
       </c>
       <c r="I45">
-        <f>[1]Inventory!H45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <f>Inventory!A46</f>
         <v>0</v>
       </c>
       <c r="I46">
-        <f>[1]Inventory!H46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <f>Inventory!A47</f>
         <v>0</v>
       </c>
       <c r="I47">
-        <f>[1]Inventory!H47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <f>Inventory!A48</f>
         <v>0</v>
       </c>
       <c r="I48">
-        <f>[1]Inventory!H48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <f>Inventory!A49</f>
         <v>0</v>
       </c>
       <c r="I49">
-        <f>[1]Inventory!H49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <f>Inventory!A50</f>
         <v>0</v>
       </c>
       <c r="I50">
-        <f>[1]Inventory!H50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <f>Inventory!A51</f>
         <v>0</v>
       </c>
       <c r="I51">
-        <f>[1]Inventory!H51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <f>Inventory!A52</f>
         <v>0</v>
       </c>
       <c r="I52">
-        <f>[1]Inventory!H52</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <f>Inventory!A53</f>
         <v>0</v>
       </c>
       <c r="I53">
-        <f>[1]Inventory!H53</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <f>Inventory!A54</f>
         <v>0</v>
       </c>
       <c r="I54">
-        <f>[1]Inventory!H54</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <f>Inventory!A55</f>
         <v>0</v>
       </c>
       <c r="I55">
-        <f>[1]Inventory!H55</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <f>Inventory!A56</f>
         <v>0</v>
       </c>
       <c r="I56">
-        <f>[1]Inventory!H56</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H56</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <f>Inventory!A57</f>
         <v>0</v>
       </c>
       <c r="I57">
-        <f>[1]Inventory!H57</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H57</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <f>Inventory!A58</f>
         <v>0</v>
       </c>
       <c r="I58">
-        <f>[1]Inventory!H58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <f>Inventory!A59</f>
         <v>0</v>
       </c>
       <c r="I59">
-        <f>[1]Inventory!H59</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <f>Inventory!A60</f>
         <v>0</v>
       </c>
       <c r="I60">
-        <f>[1]Inventory!H60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <f>Inventory!A61</f>
         <v>0</v>
       </c>
       <c r="I61">
-        <f>[1]Inventory!H61</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <f>Inventory!A62</f>
         <v>0</v>
       </c>
       <c r="I62">
-        <f>[1]Inventory!H62</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <f>Inventory!A63</f>
         <v>0</v>
       </c>
       <c r="I63">
-        <f>[1]Inventory!H63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H63</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <f>Inventory!A64</f>
         <v>0</v>
       </c>
       <c r="I64">
-        <f>[1]Inventory!H64</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <f>Inventory!A65</f>
         <v>0</v>
       </c>
       <c r="I65">
-        <f>[1]Inventory!H65</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <f>Inventory!A66</f>
         <v>0</v>
       </c>
       <c r="I66">
-        <f>[1]Inventory!H66</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <f>Inventory!A67</f>
         <v>0</v>
       </c>
       <c r="I67">
-        <f>[1]Inventory!H67</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <f>Inventory!A68</f>
         <v>0</v>
       </c>
       <c r="I68">
-        <f>[1]Inventory!H68</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <f>Inventory!A69</f>
         <v>0</v>
       </c>
       <c r="I69">
-        <f>[1]Inventory!H69</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <f>Inventory!A70</f>
         <v>0</v>
       </c>
       <c r="I70">
-        <f>[1]Inventory!H70</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H70</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <f>Inventory!A71</f>
         <v>0</v>
       </c>
       <c r="I71">
-        <f>[1]Inventory!H71</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <f>Inventory!A72</f>
         <v>0</v>
       </c>
       <c r="I72">
-        <f>[1]Inventory!H72</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H72</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <f>Inventory!A73</f>
         <v>0</v>
       </c>
       <c r="I73">
-        <f>[1]Inventory!H73</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <f>Inventory!A74</f>
         <v>0</v>
       </c>
       <c r="I74">
-        <f>[1]Inventory!H74</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H74</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <f>Inventory!A75</f>
         <v>0</v>
       </c>
       <c r="I75">
-        <f>[1]Inventory!H75</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <f>Inventory!A76</f>
         <v>0</v>
       </c>
       <c r="I76">
-        <f>[1]Inventory!H76</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <f>Inventory!A77</f>
         <v>0</v>
       </c>
       <c r="I77">
-        <f>[1]Inventory!H77</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H77</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <f>Inventory!A78</f>
         <v>0</v>
       </c>
       <c r="I78">
-        <f>[1]Inventory!H78</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H78</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <f>Inventory!A79</f>
         <v>0</v>
       </c>
       <c r="I79">
-        <f>[1]Inventory!H79</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <f>Inventory!A80</f>
         <v>0</v>
       </c>
       <c r="I80">
-        <f>[1]Inventory!H80</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <f>Inventory!A81</f>
         <v>0</v>
       </c>
       <c r="I81">
-        <f>[1]Inventory!H81</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82">
         <f>Inventory!A82</f>
         <v>0</v>
       </c>
       <c r="I82">
-        <f>[1]Inventory!H82</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83">
         <f>Inventory!A83</f>
         <v>0</v>
       </c>
       <c r="I83">
-        <f>[1]Inventory!H83</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H83</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84">
         <f>Inventory!A84</f>
         <v>0</v>
       </c>
       <c r="I84">
-        <f>[1]Inventory!H84</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85">
         <f>Inventory!A85</f>
         <v>0</v>
       </c>
       <c r="I85">
-        <f>[1]Inventory!H85</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86">
         <f>Inventory!A86</f>
         <v>0</v>
       </c>
       <c r="I86">
-        <f>[1]Inventory!H86</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H86</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87">
         <f>Inventory!A87</f>
         <v>0</v>
       </c>
       <c r="I87">
-        <f>[1]Inventory!H87</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H87</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88">
         <f>Inventory!A88</f>
         <v>0</v>
       </c>
       <c r="I88">
-        <f>[1]Inventory!H88</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H88</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89">
         <f>Inventory!A89</f>
         <v>0</v>
       </c>
       <c r="I89">
-        <f>[1]Inventory!H89</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H89</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90">
         <f>Inventory!A90</f>
         <v>0</v>
       </c>
       <c r="I90">
-        <f>[1]Inventory!H90</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91">
         <f>Inventory!A91</f>
         <v>0</v>
       </c>
       <c r="I91">
-        <f>[1]Inventory!H91</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92">
         <f>Inventory!A92</f>
         <v>0</v>
       </c>
       <c r="I92">
-        <f>[1]Inventory!H92</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93">
         <f>Inventory!A93</f>
         <v>0</v>
       </c>
       <c r="I93">
-        <f>[1]Inventory!H93</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H93</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94">
         <f>Inventory!A94</f>
         <v>0</v>
       </c>
       <c r="I94">
-        <f>[1]Inventory!H94</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H94</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95">
         <f>Inventory!A95</f>
         <v>0</v>
       </c>
       <c r="I95">
-        <f>[1]Inventory!H95</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96">
         <f>Inventory!A96</f>
         <v>0</v>
       </c>
       <c r="I96">
-        <f>[1]Inventory!H96</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97">
         <f>Inventory!A97</f>
         <v>0</v>
       </c>
       <c r="I97">
-        <f>[1]Inventory!H97</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H97</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98">
         <f>Inventory!A98</f>
         <v>0</v>
       </c>
       <c r="I98">
-        <f>[1]Inventory!H98</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99">
         <f>Inventory!A99</f>
         <v>0</v>
       </c>
       <c r="I99">
-        <f>[1]Inventory!H99</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H99</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100">
         <f>Inventory!A100</f>
         <v>0</v>
       </c>
       <c r="I100">
-        <f>[1]Inventory!H100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101">
         <f>Inventory!A101</f>
         <v>0</v>
       </c>
       <c r="I101">
-        <f>[1]Inventory!H101</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H101</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102">
         <f>Inventory!A102</f>
         <v>0</v>
       </c>
       <c r="I102">
-        <f>[1]Inventory!H102</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H102</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103">
         <f>Inventory!A103</f>
         <v>0</v>
       </c>
       <c r="I103">
-        <f>[1]Inventory!H103</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H103</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104">
         <f>Inventory!A104</f>
         <v>0</v>
       </c>
       <c r="I104">
-        <f>[1]Inventory!H104</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H104</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105">
         <f>Inventory!A105</f>
         <v>0</v>
       </c>
       <c r="I105">
-        <f>[1]Inventory!H105</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H105</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106">
         <f>Inventory!A106</f>
         <v>0</v>
       </c>
       <c r="I106">
-        <f>[1]Inventory!H106</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H106</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107">
         <f>Inventory!A107</f>
         <v>0</v>
       </c>
       <c r="I107">
-        <f>[1]Inventory!H107</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H107</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108">
         <f>Inventory!A108</f>
         <v>0</v>
       </c>
       <c r="I108">
-        <f>[1]Inventory!H108</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H108</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109">
         <f>Inventory!A109</f>
         <v>0</v>
       </c>
       <c r="I109">
-        <f>[1]Inventory!H109</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H109</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110">
         <f>Inventory!A110</f>
         <v>0</v>
       </c>
       <c r="I110">
-        <f>[1]Inventory!H110</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H110</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111">
         <f>Inventory!A111</f>
         <v>0</v>
       </c>
       <c r="I111">
-        <f>[1]Inventory!H111</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H111</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112">
         <f>Inventory!A112</f>
         <v>0</v>
       </c>
       <c r="I112">
-        <f>[1]Inventory!H112</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H112</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113">
         <f>Inventory!A113</f>
         <v>0</v>
       </c>
       <c r="I113">
-        <f>[1]Inventory!H113</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H113</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114">
         <f>Inventory!A114</f>
         <v>0</v>
       </c>
       <c r="I114">
-        <f>[1]Inventory!H114</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H114</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115">
         <f>Inventory!A115</f>
         <v>0</v>
       </c>
       <c r="I115">
-        <f>[1]Inventory!H115</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H115</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116">
         <f>Inventory!A116</f>
         <v>0</v>
       </c>
       <c r="I116">
-        <f>[1]Inventory!H116</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H116</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117">
         <f>Inventory!A117</f>
         <v>0</v>
       </c>
       <c r="I117">
-        <f>[1]Inventory!H117</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H117</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118">
         <f>Inventory!A118</f>
         <v>0</v>
       </c>
       <c r="I118">
-        <f>[1]Inventory!H118</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H118</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119">
         <f>Inventory!A119</f>
         <v>0</v>
       </c>
       <c r="I119">
-        <f>[1]Inventory!H119</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H119</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120">
         <f>Inventory!A120</f>
         <v>0</v>
       </c>
       <c r="I120">
-        <f>[1]Inventory!H120</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+        <f ca="1">[1]Inventory!H120</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121">
         <f>Inventory!A121</f>
         <v>0</v>
       </c>
       <c r="I121">
-        <f>[1]Inventory!H121</f>
+        <f ca="1">[1]Inventory!H121</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>